<commit_message>
add maven.lib and put index
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -818,6 +818,21 @@
         }
     }
 }</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Java Command Line</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>To call a java program on a command line, there are 2 ways:
+1. Call the runnable jar: &gt;java -jar NameOfJar.jar arg1 arg2...
+2. Call the class: &gt;java -cp {jar_path} com.myles.ClassName 
+arg1 arg2...</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1308,21 +1323,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1333,7 +1348,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1344,7 +1359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1355,7 +1370,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -1366,7 +1381,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1377,7 +1392,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1403,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1399,7 +1414,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1410,7 +1425,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1421,7 +1436,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -1432,7 +1447,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1443,7 +1458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1454,7 +1469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1465,7 +1480,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1476,7 +1491,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1487,7 +1502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1498,7 +1513,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -1509,7 +1524,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -1520,7 +1535,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1531,7 +1546,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
@@ -1539,7 +1554,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -1550,7 +1565,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>97</v>
       </c>
@@ -1559,6 +1574,17 @@
       </c>
       <c r="C22" s="2" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1575,65 +1601,65 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="77.375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="93.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>66</v>
       </c>
@@ -1647,7 +1673,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>70</v>
       </c>
@@ -1661,7 +1687,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>74</v>
       </c>
@@ -1675,7 +1701,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>76</v>
       </c>
@@ -1689,7 +1715,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>79</v>
       </c>
@@ -1703,7 +1729,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>81</v>
       </c>
@@ -1717,7 +1743,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>85</v>
       </c>
@@ -1731,7 +1757,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>89</v>
       </c>
@@ -1745,7 +1771,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="46.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>92</v>
       </c>
@@ -1759,7 +1785,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>95</v>
       </c>
@@ -1787,7 +1813,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add gfatca new version
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="110">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -835,36 +835,99 @@
 arg1 arg2...</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>Basic CI &amp; SI</t>
+  </si>
+  <si>
+    <t>Below xml is a whole xml contains basic contructor injection and setter injection:
+------------------------------------------------------------------------------------------------------------------
+&lt;beans xmlns="http://www.springframework.org/schema/beans"
+ xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"
+ xsi:schemaLocation="http://www.springframework.org/schema/beans
+ http://www.springframework.org/schema/beans/spring-beans-3.0.xsd"&gt;
+  &lt;bean id="helloBean" class="com.bcm.client.HelloWorld"&gt;
+    &lt;property name="name" value="Myles" /&gt;
+  &lt;/bean&gt;
+  &lt;bean id="frameBean" class="javax.swing.JFrame"&gt;
+    &lt;constructor-arg value="Demo-Screen" /&gt;
+  &lt;/bean&gt;
+  &lt;bean id="panelBean" class="javax.swing.JPanel" /&gt;
+  &lt;bean id="layoutBean" class="java.awt.FlowLayout" /&gt;
+  &lt;bean id="labelBean" class="javax.swing.JLabel"&gt;
+    &lt;constructor-arg value="This is the label." /&gt;
+  &lt;/bean&gt;
+  &lt;bean id="buttonBean" class="javax.swing.JButton" /&gt;
+&lt;/beans&gt;</t>
+  </si>
+  <si>
+    <t>Make a swing component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">package com.bcm.client;
+import org.springframework.context.ApplicationContext;
+import org.springframework.context.support.ClassPathXmlApplicationContext;
+import com.bcm.client.autopay.collection.*;
+import javax.swing.*;
+import java.awt.FlowLayout;
+import javax.swing.*;
+public class Launcher {
+  public static void main(String[] args) {
+    ApplicationContext context = new ClassPathXmlApplicationContext("SpringBeans.xml");
+// inject for a custom bean object
+    HelloWorld obj1 = (HelloWorld) context.getBean("helloBean");
+    obj1.printHello();
+// inject for a jframe and its components
+    JFrame frame = (JFrame) context.getBean("frameBean");
+    JPanel panel = (JPanel) context.getBean("panelBean");
+    FlowLayout layout = (FlowLayout) context.getBean("layoutBean");
+    JLabel label = (JLabel) context.getBean("labelBean");
+    JButton button = (JButton) context.getBean("buttonBean");
+ panel.setLayout(layout);
+ button.setText("Press me");
+ panel.add(label);
+ panel.add(button);
+ frame.add(panel);
+ frame.setSize(300, 300);
+ frame.setLocationRelativeTo(null);
+ frame.setDefaultCloseOperation(JFrame.EXIT_ON_CLOSE);
+ frame.setVisible(true);
+ }
+}
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1023,8 +1086,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1037,7 +1100,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1111,7 +1174,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1146,7 +1208,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1322,22 +1383,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="3"/>
+    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="33" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1348,7 +1409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1359,7 +1420,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1370,7 +1431,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -1381,7 +1442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1392,7 +1453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1403,7 +1464,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1414,7 +1475,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1425,7 +1486,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="33" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1436,7 +1497,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="33" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -1447,7 +1508,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="33" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1458,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="33" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1530,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="33" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1480,7 +1541,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="33" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1491,7 +1552,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="33" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1502,7 +1563,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="33" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1513,7 +1574,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="33" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -1524,7 +1585,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="33" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -1535,7 +1596,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="33" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1546,7 +1607,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="33" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
@@ -1554,7 +1615,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="33" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -1565,7 +1626,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="33" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>97</v>
       </c>
@@ -1576,7 +1637,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="33" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>102</v>
       </c>
@@ -1585,6 +1646,28 @@
       </c>
       <c r="C23" s="2" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="33" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="33" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1594,72 +1677,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="77.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="37.5">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="93.75">
       <c r="A5" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="60">
       <c r="A13" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="39">
       <c r="A15" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="10" t="s">
         <v>66</v>
       </c>
@@ -1673,7 +1756,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
         <v>70</v>
       </c>
@@ -1687,7 +1770,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
         <v>74</v>
       </c>
@@ -1701,7 +1784,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="12" t="s">
         <v>76</v>
       </c>
@@ -1715,7 +1798,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="11" t="s">
         <v>79</v>
       </c>
@@ -1729,7 +1812,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
         <v>81</v>
       </c>
@@ -1743,7 +1826,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="30">
       <c r="A23" s="11" t="s">
         <v>85</v>
       </c>
@@ -1757,7 +1840,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
         <v>89</v>
       </c>
@@ -1771,7 +1854,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="43.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="46.5">
       <c r="A25" s="11" t="s">
         <v>92</v>
       </c>
@@ -1785,7 +1868,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="30">
       <c r="A26" s="11" t="s">
         <v>95</v>
       </c>
@@ -1808,12 +1891,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Add mvn ref pom for runnable jar and exe building 2. Add index entry introducing Refactoring / Martin Fowler 3. Add java note for file inputing for java utilities programming
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="112">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -897,6 +897,13 @@
  }
 }
 </t>
+  </si>
+  <si>
+    <t>Get the current working path</t>
+  </si>
+  <si>
+    <t>用System 句柄
+String workingDirectory = System.getProperty("user.dir");</t>
   </si>
 </sst>
 </file>
@@ -1384,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
@@ -1668,6 +1675,17 @@
       </c>
       <c r="C25" s="2" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="33" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
setup page in java lib to record source code reading journey
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="jdbc  connection properties" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="the source" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="115">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -904,6 +904,15 @@
   <si>
     <t>用System 句柄
 String workingDirectory = System.getProperty("user.dir");</t>
+  </si>
+  <si>
+    <t>Source code of JDK 1.8 reading practice note/</t>
+  </si>
+  <si>
+    <t>keyword "default" is added in jdk8 to extend interfaces to adopt lambda expression. So that adding new method in interface wont break the compilation and running of java code in new jre. E.g java.util.Collection</t>
+  </si>
+  <si>
+    <t>read java.lang.Boolean</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1064,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1091,6 +1100,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1393,7 +1403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1910,12 +1920,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="82.5703125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45">
+      <c r="A3" s="13">
+        <v>42772</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="13">
+        <v>42772</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add JPA convept, Spring-boot concept, JSR intro, some cheatsheet and the usage of plugin tag in mvn pom
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -956,36 +956,138 @@
    }
   }</t>
   </si>
+  <si>
+    <t>JPA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPA Basics:</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. We use annoation @Entity(name="EntityName") to define a class as entity which its instance is a row in the relational database tables.
+2. @Table(name=”TABLE_NAME”) &gt; JPA will create a database table with name TABLE_NAME, but @Entity also creates a database table, so @Table is optional.
+3. @Transient any field within an entity will not be persisted so no database table column will be created
+4. @Version for concurrent modification and optimistic locking
+5. @Id we can define the primary key
+6. @GeneratedValue we can specify that the database is going to generate the value for the given field. Usually set strategyType = AUTO for id.
+7. The EntityManager is like the role of contextManager in Spring. We manipulate entities with the manager, we have method: persist(), remove(), merge(), delete() from the manager.
+8. JPA support SQL, but it also has its own JPQL, which is Entity-Oriented.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. JPA is the standard specification and Hibernate/EclipseLink are the vendor who actually produce the implementing tools. 
+2. In JPA, we config the persistence.xml to specify which vendor we are going to use. 
+3. Sometimes we use Hibernate directly because JPA does not support specific feature yet. How? Change some import path from points at JPA to points at Hibernate.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPA vs. Hibernate</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spring web example (case from udemy course)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spring Boot Concept</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spring-boot</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Spring is design to fasten the building of Spring application and its of course base on spring (btw, spring is build upon the vision that allow people to build software at a easier way with higher quality)
+2. Spring boot also package tomcat, jboss, jetty into itself thus enabling an awesome simple way to build micro-service.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* pom:
+  - specifies the dependency of spring-boot-starter-web and spring-boot-starter-tomcat
+  - the packaging tag with war value. 
+  - build&gt;plugin&gt;spring-boot-maven-plugin&gt;executable&gt;true
+* Student Class:
+  - defined with @Component annoation
+  - has a private Address member to which we put @Autowired annoation
+* Address Class:
+  - defined with @Component annoation
+* In App class(the entrance class)
+  - @EnableAutoConfiguration, @RestController, @ComponentScan, 3 annoations are attached to Class App.
+  - its private member Student has an @Autowired
+  - it has hello method with @RequestMapping("/index")
+* $mvn package &amp;&amp; mvn spring-boot:run 
+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. JSR stands for Java Specification Request, it defines the "Floorplan" of the java language.
+2. JCP (Java Community Process) has 4 major steps that renew the JSR:
+ i) Initiation: A specification is initiated by community members and approved for development by the Executive Committee. At times, there are new JSRs being accepted every week. 
+ ii) Draft Releases: Once a JSR is approved, a group of experts is formed to develop a progressive drafts of the specification that anyone with an internet connection can review. 
+ iii) Final Release: The Expert Group uses the public feedback to further revise the document into a Proposed Final Draft...Once approved, the final Specification, Reference Implementation and Technology Compatibility Kit are published, and the Specification Lead arranges for a Maintenance Lead.
+ iv) Maintenance: The Maintenance Lead tracks requests for clarification, interpretation, enhancements and revisions in an Issue Tracker... until the specification can be revised by an Expert Group in a new JSR. 
+3. Currently the EC(Executive Committee) include big names like: Azul, Eclipse Foundation, Fujitsu, Goldman Sachs, HP, IBM, Intel, Oracle, RedHat, SAP, Twitter...</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSR Concepts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSR Concepts (2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oracle為Java 提供實現JSR的lib或其他工具, 但如果其他Vendor有意, 也可制作可滿足該JSR的lib. 這就像JPA定義了接口, Hibernate來實現, 又例如JDBC的接口, 各大DB Vendor各自提供JDBC Connector</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encryption</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Popular Libs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">JaSypt amd bouncy castle </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1148,8 +1250,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1162,7 +1264,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="index"/>
@@ -1199,7 +1301,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1273,6 +1375,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1307,6 +1410,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1482,22 +1586,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1">
+    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>30</v>
       </c>
@@ -1508,7 +1612,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1519,7 +1623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1530,7 +1634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -1541,7 +1645,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1552,7 +1656,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -1563,7 +1667,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1574,7 +1678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1585,7 +1689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" customHeight="1">
+    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1596,7 +1700,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="33" customHeight="1">
+    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>28</v>
       </c>
@@ -1607,7 +1711,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1">
+    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -1618,7 +1722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33" customHeight="1">
+    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1629,7 +1733,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="33" customHeight="1">
+    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1640,7 +1744,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1">
+    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -1651,7 +1755,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="33" customHeight="1">
+    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1662,7 +1766,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1">
+    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>42</v>
       </c>
@@ -1673,7 +1777,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="33" customHeight="1">
+    <row r="17" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -1684,7 +1788,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="33" customHeight="1">
+    <row r="18" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -1695,7 +1799,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1">
+    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1706,7 +1810,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="33" customHeight="1">
+    <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
@@ -1714,7 +1818,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33" customHeight="1">
+    <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>97</v>
       </c>
@@ -1725,7 +1829,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33" customHeight="1">
+    <row r="22" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>97</v>
       </c>
@@ -1736,7 +1840,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="33" customHeight="1">
+    <row r="23" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>102</v>
       </c>
@@ -1747,7 +1851,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="33" customHeight="1">
+    <row r="24" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>105</v>
       </c>
@@ -1758,7 +1862,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="33" customHeight="1">
+    <row r="25" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>105</v>
       </c>
@@ -1769,7 +1873,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="33" customHeight="1">
+    <row r="26" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1780,7 +1884,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="33" customHeight="1">
+    <row r="27" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
@@ -1789,6 +1893,83 @@
       </c>
       <c r="C27" s="2" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1799,72 +1980,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="77.375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="37.5">
+    <row r="1" spans="1:1" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75">
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="93.75">
+    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75">
+    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75">
+    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75">
+    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75">
+    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="60">
+    <row r="13" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="39">
+    <row r="15" spans="1:1" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>66</v>
       </c>
@@ -1878,7 +2059,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>70</v>
       </c>
@@ -1892,7 +2073,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>74</v>
       </c>
@@ -1906,7 +2087,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>76</v>
       </c>
@@ -1920,7 +2101,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>79</v>
       </c>
@@ -1934,7 +2115,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>81</v>
       </c>
@@ -1948,7 +2129,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
+    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>85</v>
       </c>
@@ -1962,7 +2143,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>89</v>
       </c>
@@ -1976,7 +2157,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="46.5">
+    <row r="25" spans="1:4" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>92</v>
       </c>
@@ -1990,7 +2171,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>95</v>
       </c>
@@ -2013,25 +2194,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="82.5703125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="82.625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A3" s="13">
         <v>42772</v>
       </c>
@@ -2039,7 +2220,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>42772</v>
       </c>
@@ -2047,7 +2228,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>42754</v>
       </c>

</xml_diff>

<commit_message>
Add java entry on JPA quick fact
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="139">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -965,23 +965,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1. We use annoation @Entity(name="EntityName") to define a class as entity which its instance is a row in the relational database tables.
-2. @Table(name=”TABLE_NAME”) &gt; JPA will create a database table with name TABLE_NAME, but @Entity also creates a database table, so @Table is optional.
-3. @Transient any field within an entity will not be persisted so no database table column will be created
-4. @Version for concurrent modification and optimistic locking
-5. @Id we can define the primary key
-6. @GeneratedValue we can specify that the database is going to generate the value for the given field. Usually set strategyType = AUTO for id.
-7. The EntityManager is like the role of contextManager in Spring. We manipulate entities with the manager, we have method: persist(), remove(), merge(), delete() from the manager.
-8. JPA support SQL, but it also has its own JPQL, which is Entity-Oriented.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. JPA is the standard specification and Hibernate/EclipseLink are the vendor who actually produce the implementing tools. 
-2. In JPA, we config the persistence.xml to specify which vendor we are going to use. 
-3. Sometimes we use Hibernate directly because JPA does not support specific feature yet. How? Change some import path from points at JPA to points at Hibernate.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>JPA vs. Hibernate</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1058,12 +1041,73 @@
     <t xml:space="preserve">JaSypt amd bouncy castle </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>1. We use annoation @Entity(name="EntityName") to define a class as entity which its instance is a row in the relational database tables.
+2. @Table(name=”TABLE_NAME”) &gt; JPA will create a database table with name TABLE_NAME, but @Entity also creates a database table, so @Table is optional.
+3. @Transient any field within an entity will not be persisted so no database table column will be created
+4. @Version for concurrent modification and optimistic locking
+5. @Id we can define the primary key
+6. @GeneratedValue we can specify that the database is going to generate the value for the given field. Usually set strategyType = AUTO for id.
+7. The EntityManager is like the role of contextManager in Spring. We manipulate entities with the manager, we have method: persist(), remove(), merge(), delete() from the manager.
+8. JPA support SQL, but it also has its own JPQL, which is Entity-Oriented.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. JPA is the standard specification and Hibernate/EclipseLink are the vendor who actually produce the implementing tools. 
+2. In JPA, we config the persistence.xml to specify which vendor we are going to use. 
+3. Sometimes we use Hibernate directly because JPA does not support specific feature yet. How? Change some import path from points at JPA to points at Hibernate.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JPA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quick facts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># JDBC rely on SQL, while new approach like JPA, Hibernate, EclipseLink, are more user-friendly.
+# JPA base on JDBC in bg.
+# JPA is the API providers. Such as EclipseLink and Hibernate define the concrete impl for the JPA specification.
+# 2 ways to specify the ORM impl, the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>orm.xml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or the annotation (@Entity, @Table, @Id, @Transient, @OnetoMany, @ManytoMany)
+# Dependency for a simple JPA project can be: 
+  - mysql-connector 
+  - hibernate jpa
+  - hibernate core
+  - hibernate entity manager</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1149,6 +1193,15 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1587,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1903,7 +1956,7 @@
         <v>119</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -1911,71 +1964,82 @@
         <v>118</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add java entries on JAD (java decompiler) and Jacob (java com bridge)
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,14 +15,14 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="TagOptions">[1]options!$B$2:$B$4</definedName>
+    <definedName name="TagOptions">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="142">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -111,11 +111,6 @@
         System.out.println("Click Detected by Anon Class");
     }
 });</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>import org.apache.commona.io.FileUtils;
-String fileContent=FileUtils.readFileToString(file);</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -1058,36 +1053,64 @@
     <t xml:space="preserve">JaSypt amd bouncy castle </t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>JAD</t>
+  </si>
+  <si>
+    <t>The apache is so comvenient that most of the move, copy, delete work can be performed without instantializing the File class:
+$ import org.apache.commona.io.FileUtils;
+$ String fileContent=FileUtils.readFileToString(file);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java Decompiler </t>
+  </si>
+  <si>
+    <t>When you want to reverse a java class file to java source file, use:
+$jad {target_class}.class 
+And the jad will generate {target_class}.jad file which is a java file
+There are version constraint for jad, refers to:
+http://www.javadecompilers.com/jad</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>A dll calling project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JACOB is a JAVA-COM Bridge that allows you to call COM Automation components from Java. It uses JNI to make native calls to the COM libraries. JACOB runs on x86 and x64 environments supporting 32 bit and 64 bit JVMs
+( https://github.com/joval/jacob ) </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1250,8 +1273,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1264,44 +1287,38 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="index"/>
-      <sheetName val="options"/>
-      <sheetName val="AS400 Version"/>
-      <sheetName val="Apache Overview"/>
-      <sheetName val="Apache Details"/>
+      <sheetName val="g2k"/>
+      <sheetName val="pf meaning"/>
+      <sheetName val="imodule"/>
+      <sheetName val="CFSORC"/>
+      <sheetName val="icbs_utility"/>
+      <sheetName val="in-house"/>
+      <sheetName val="SRP"/>
+      <sheetName val="as400 cust-option"/>
+      <sheetName val="doom_code"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>#concept</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>#resource</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>#fact</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1375,7 +1392,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1410,7 +1426,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1586,24 +1601,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="3"/>
+    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="33" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1612,9 +1627,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -1623,20 +1638,20 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -1645,42 +1660,42 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -1689,31 +1704,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="33" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="33" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="33" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -1722,254 +1737,276 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="33" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="33" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="33" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="33" customHeight="1">
+      <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="33" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="33" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="33" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="33" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="33" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="33" customHeight="1">
       <c r="A21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="33" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="33" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="33" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="33" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="33" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" ht="33" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="33" customHeight="1">
+      <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="33" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="30" spans="1:3" ht="33" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="71.45" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C31" s="2" t="s">
+    <row r="32" spans="1:3" ht="33" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:3" ht="33" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:3" ht="33" customHeight="1">
+      <c r="A34" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:3" ht="33" customHeight="1">
+      <c r="A35" s="2" t="s">
         <v>135</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="33" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1980,207 +2017,207 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="77.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="37.5">
       <c r="A1" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75">
+      <c r="A3" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+    <row r="5" spans="1:1" ht="93.75">
+      <c r="A5" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+    <row r="7" spans="1:1" ht="15.75">
+      <c r="A7" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+    <row r="8" spans="1:1" ht="15.75">
+      <c r="A8" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+    <row r="9" spans="1:1" ht="15.75">
+      <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+    <row r="10" spans="1:1" ht="15.75">
+      <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:1" ht="15.75">
+      <c r="A11" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
+    <row r="13" spans="1:1" ht="60">
+      <c r="A13" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="15" spans="1:1" ht="39">
+      <c r="A15" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="53.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="10" t="s">
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="12" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="11" t="s">
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="B19" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="11" t="s">
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="11" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="15.75">
+      <c r="A21" s="11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="B21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="11" t="s">
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="11" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+      <c r="B22" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="11" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="30">
+      <c r="A23" s="11" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="11" t="s">
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="11" t="s">
+      <c r="B24" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="C24" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" s="11" t="s">
+    </row>
+    <row r="25" spans="1:4" ht="46.5">
+      <c r="A25" s="11" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="43.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+      <c r="B25" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C25" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="11" t="s">
+    </row>
+    <row r="26" spans="1:4" ht="30">
+      <c r="A26" s="11" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
-        <v>95</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2194,46 +2231,46 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="82.625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="82.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45">
       <c r="A3" s="13">
         <v>42772</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="13">
         <v>42772</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45">
       <c r="A5" s="14">
         <v>42754</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>

</xml_diff>

<commit_message>
Add entres about Cookie, Session, and JVM optimization
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="150">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1118,6 +1118,71 @@
   <si>
     <t xml:space="preserve">JACOB is a JAVA-COM Bridge that allows you to call COM Automation components from Java. It uses JNI to make native calls to the COM libraries. JACOB runs on x86 and x64 environments supporting 32 bit and 64 bit JVMs_x000D_
 ( https://github.com/joval/jacob ) </t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Cookie</t>
+  </si>
+  <si>
+    <t>Cookie
+1. The goal is to provide extra knowledge in a httprequest to server
+2. The agreement is that server issued Cookie in httpresponse and browser saved it locally and pack it with new httprequest afterward
+3. Two types of cookies in servlets:
+    * Non-persistent ck: valid for single session only. It is removed each time when user closes the browser
+    * Persistent ck: valid for multiple session . It is not removed each time when user closes the browser. It is removed only if user logout or signout.
+4. How to set cookie to httpresponse (At server side):
+    $ ...
+    $ Cookie loginCookie = new Cookie("user",user);
+    $ loginCookie.setMaxAge(30*60);     //set cookie expiry in 30 mins
+    $ response.addCookie(loginCookie);
+    $ response.sendRedirect("LoginSuccess.jsp");
+    $ ...
+5. How to read Cookie (At server side):
+    $ ...
+    $ Cookie[] cookies = request.getCookies();
+    $ if(cookies != null){
+    $   for(Cookie cookie : cookies){
+    $     if(cookie.getName().equals("user")) userName = cookie.getValue();
+    $ ...</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Session?
+1. HTTP protocol and Web Servers are stateless, what it means is that for web server every request is a new request to process and they can’t identify if it’s coming from client that has been sending request previously. So comes the Session concept.
+2. Session vs. Cookie:
+    * Session at Server side / Cookie at client (browser) side
+    * Session is a concept impl by Cookie / Cookie is physical at client (browser) side
+3. How to set Session to httpresponse (At server side):
+ $ if(userID.equals(user) &amp;&amp; password.equals(pwd)){
+ $  HttpSession session = request.getSession();
+ $  session.setAttribute("user", "Pankaj");
+ $  session.setMaxInactiveInterval(30*60); //setting session to expiry in 30 mins
+ $  Cookie userName = new Cookie("user", user);
+ $  userName.setMaxAge(30*60);
+ $  response.addCookie(userName);
+ $  response.sendRedirect("LoginSuccess.jsp");
+    $ ...
+4. How to read Session info (At server side):
+    $ if(session.getAttribute("user") == null){
+    $   response.sendRedirect("login.html");
+    $ }else{
+    $   user = (String) session.getAttribute("user");
+    $ }
+    $ String userName = null;
+    $ String sessionID = null;
+    $ Cookie[] cookies = request.getCookies();
+    $ if(cookies !=null){
+    $   for(Cookie cookie : cookies){
+    $       if(cookie.getName().equals("user")) userName = cookie.getValue();
+    $       if(cookie.getName().equals("JSESSIONID")) sessionID = cookie.getValue();
+    $   }
+    $ }
+5. The session data is stored on server side, usually in text files in a temporary directory. They can not be accessed from outside. The thing connecting a session to a client browser is the session ID, which is usually stored in a cookie. This ID is, and should be, the only thing about your session that is stored on client side.
+</t>
   </si>
 </sst>
 </file>
@@ -1616,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
@@ -2032,6 +2097,28 @@
       </c>
       <c r="C37" s="2" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="33" customHeight="1">
+      <c r="A38" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="33" customHeight="1">
+      <c r="A39" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry on spring-boot
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="214">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -2094,24 +2094,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">* pom:
-  - specifies the dependency of spring-boot-starter-web and spring-boot-starter-tomcat
-  - the packaging tag with war value. 
-  - build&gt;plugin&gt;spring-boot-maven-plugin&gt;executable&gt;true
-* Student Class:
-  - defined with @Component annoation
-  - has a private Address member to which we put @Autowired annoation
-* Address Class:
-  - defined with @Component annoation
-* In App class(the entrance class)
-  - @EnableAutoConfiguration, @RestController, @ComponentScan, 3 annoations are attached to Class App.
-  - its private member Student has an @Autowired
-  - it has hello method with @RequestMapping("/index")
-* $mvn package &amp;&amp; mvn spring-boot:run 
-</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Spring-boot</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2137,12 +2119,6 @@
   </si>
   <si>
     <t>Official Guide: jar-&gt; war</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>大體上猜測2個主要設計特性:
-1. 將含Main Method的Class 掃描出來, 當做是總設置(General Configuration)
-2. 在Maven Dependency中加入的spring-boot-starter-xxx 再不是被動的, 而是一旦安裝上去了, 就會有相關的configurator去主動查你的App 是否有進行相應主題的Annotation設置, 若找不到需要的Annotation則報錯(比如在Udemy上我跟著設JPA時的錯)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -2413,6 +2389,39 @@
     - 85.1 Create a deployable war file
 * 特別的是, 在做完這個處理後, 不單war檔可以交由tomcat/jboss運行, 也可以java -jar它來運行.</t>
     </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">* pom:
+  - specifies the dependency of spring-boot-starter-web and spring-boot-starter-tomcat
+  - the packaging tag with war value. 
+  - build&gt;plugin&gt;spring-boot-maven-plugin&gt;executable&gt;true
+* Student Class:
+  - defined with @Component annoation
+  - has a private Address member to which we put @Autowired annoation
+* Address Class:
+  - defined with @Component annoation
+* In App class(the entrance class)
+  - @EnableAutoConfiguration, @RestController, @ComponentScan, 3 annoations are attached to Class App.
+  - its private member Student has an @Autowired
+  - it has hello method with @RequestMapping("/index")
+* $mvn package &amp;&amp; mvn spring-boot:run 
+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>大體上猜測2個主要設計特性:
+1. 將含Main Method的Class 掃描出來, 當做是總設置(General Configuration)
+2. 在Maven Dependency中加入的spring-boot-starter-xxx 再不是被動的, 而是一旦安裝上去了, 就會有相關的configurator去主動查你的App 是否有進行相應主題的Annotation設置, 若找不到需要的Annotation則報錯(比如在Udemy上我跟著設JPA時的錯)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Organization Understanding Assumsion (2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>驗證了猜測: dependency 在Spring boot的世界中的確是主動的, 我在項目中加入了spring-boot-starter-data-jpa, Compile 沒有問題, 但當run jar時, Spring報錯: org.springframework.beans.factory.BeanCreationException: Error creating bean with name 'org.s…
+很可能是因為Autowire不到dependency 所需的類所以報錯.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2922,10 +2931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3546,73 +3555,84 @@
         <v>122</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="C57" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B60" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>204</v>
-      </c>
       <c r="C60" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>209</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry on springboot x GUI and the philosophy
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="223">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1050,7 +1050,7 @@
         <b/>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1061,7 +1061,7 @@
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2089,11 +2089,6 @@
 }</t>
   </si>
   <si>
-    <t>1. Spring is design to fasten the building of Spring application and its of course base on spring (btw, spring is build upon the vision that allow people to build software at a easier way with higher quality)
-2. Spring boot also package tomcat, jboss, jetty into itself thus enabling an awesome simple way to build micro-service.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Spring-boot</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2253,15 +2248,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>@SpringBootApplication is a convenience annotation that adds all of the following:
-1. @Configuration tags the class as a source of bean definitions for the application context.
-2. @EnableAutoConfiguration tells Spring Boot to start adding beans based on classpath settings, other beans, and various property settings.
-3. Normally you would add @EnableWebMvc for a Spring MVC app, but Spring Boot adds it automatically when it sees spring-webmvc on the classpath. This flags the application as a web application and activates key behaviors such as setting up a DispatcherServlet.
-4. @ComponentScan tells Spring to look for other components, configurations, and services in the  hello package, allowing it to find the controllers.
-The main() method uses Spring Boot’s SpringApplication.run() method to launch an application. Did you notice that there wasn’t a single line of XML? No web.xml file either. This web application is 100% pure Java and you didn’t have to deal with configuring any plumbing or infrastructure.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">1. POM Paraent/ Dpdncy/ Build:
     &lt;parent&gt;
         &lt;groupId&gt;org.springframework.boot&lt;/groupId&gt;
@@ -2352,7 +2338,7 @@
         <b/>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2363,7 +2349,7 @@
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2390,6 +2376,17 @@
 * 特別的是, 在做完這個處理後, 不單war檔可以交由tomcat/jboss運行, 也可以java -jar它來運行.</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Organization Understanding Assumsion (2)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spring-boot</t>
+  </si>
+  <si>
+    <t>1. Spring is design to fasten the building of Spring application and its of course base on spring (btw, spring is build upon the vision that allow people to build software at a easier way with higher quality)
+2. Spring boot also package tomcat, jboss, jetty into itself thus enabling an awesome simple way to build micro-service.</t>
   </si>
   <si>
     <t xml:space="preserve">* pom:
@@ -2407,53 +2404,117 @@
   - it has hello method with @RequestMapping("/index")
 * $mvn package &amp;&amp; mvn spring-boot:run 
 </t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>大體上猜測2個主要設計特性:
 1. 將含Main Method的Class 掃描出來, 當做是總設置(General Configuration)
 2. 在Maven Dependency中加入的spring-boot-starter-xxx 再不是被動的, 而是一旦安裝上去了, 就會有相關的configurator去主動查你的App 是否有進行相應主題的Annotation設置, 若找不到需要的Annotation則報錯(比如在Udemy上我跟著設JPA時的錯)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Organization Understanding Assumsion (2)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>@SpringBootApplication is a convenience annotation that adds all of the following:
+1. @Configuration tags the class as a source of bean definitions for the application context.
+2. @EnableAutoConfiguration tells Spring Boot to start adding beans based on classpath settings, other beans, and various property settings.
+3. Normally you would add @EnableWebMvc for a Spring MVC app, but Spring Boot adds it automatically when it sees spring-webmvc on the classpath. This flags the application as a web application and activates key behaviors such as setting up a DispatcherServlet.
+4. @ComponentScan tells Spring to look for other components, configurations, and services in the  hello package, allowing it to find the controllers.
+The main() method uses Spring Boot’s SpringApplication.run() method to launch an application. Did you notice that there wasn’t a single line of XML? No web.xml file either. This web application is 100% pure Java and you didn’t have to deal with configuring any plumbing or infrastructure.</t>
   </si>
   <si>
     <t>驗證了猜測: dependency 在Spring boot的世界中的確是主動的, 我在項目中加入了spring-boot-starter-data-jpa, Compile 沒有問題, 但當run jar時, Spring報錯: org.springframework.beans.factory.BeanCreationException: Error creating bean with name 'org.s…
 很可能是因為Autowire不到dependency 所需的類所以報錯.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>More on Spring-boot IoC</t>
+  </si>
+  <si>
+    <t>Non-web application (1)</t>
+  </si>
+  <si>
+    <t>Non-web application (3) - Swing GUI</t>
+  </si>
+  <si>
+    <t>Non-web application (2) - Method Bean as Entrance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">package hello;
+import java.util.Arrays;
+import org.springframework.boot.CommandLineRunner;
+import org.springframework.boot.SpringApplication;
+import org.springframework.boot.autoconfigure.SpringBootApplication;
+import org.springframework.context.ApplicationContext;
+import org.springframework.context.annotation.Bean;
+@SpringBootApplication
+public class Application {
+    public static void main(String[] args) {
+        SpringApplication.run(Application.class, args);
+    }
+    @Bean
+    public CommandLineRunner commandLineRunner(ApplicationContext ctx) {
+        return args -&gt; {
+            System.out.println("Let's inspect the beans provided by Spring Boot:");
+            String[] beanNames = ctx.getBeanDefinitionNames();
+            Arrays.sort(beanNames);
+            for (String beanName : beanNames) {
+                System.out.println(beanName);
+            }
+        };
+    }
+}
+</t>
+  </si>
+  <si>
+    <t>There is an code sample on github provided:
+https://kemitix.wordpress.com/2015/03/24/creating-an-awt-or-swing-gui-application-with-spring-boot/</t>
+  </si>
+  <si>
+    <t>2 blogs talks details of springboot DI operation:
+a) Part1 on What is starters:  https://stormpath.com/blog/spring-boot-default-starters
+b) Part2 on How to DI: https://stormpath.com/blog/spring-boot-dependency-injection</t>
+  </si>
+  <si>
+    <t>Both Spring boot and Spring support non-web application, but they invoke the target classes in different way due to their design purpose:
+1. In traditional spring, we use the main method as entrance and start our logic like below:
+    public void main(...){
+        ApplicationContext context = ...
+        myBean = context.getBean(....
+2. In springboot, since the framework use the main as the configuration, the philosophy is changed upside down, everything is passive 被動地被框架調用(like the restcontroller, or scheduletask). So we can no longer add our login in main after the SpringApplication.run(...) because if we want to run any code, we need to find the suitable @annotation which can inform the framework on the time we want it to be invoked. And the simplest way is @Bean for method after the main method:
+    public void main(...){
+        SpringApplication.run(...);
+    }
+    @Bean
+    public JFrame invokeFrame(){
+        return new CustomFrame();
+    }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2520,7 +2581,7 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2631,8 +2692,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2645,7 +2706,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2719,7 +2780,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2754,7 +2814,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2930,22 +2989,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="3"/>
+    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="33" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -2956,7 +3015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -2967,7 +3026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -2978,7 +3037,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -2989,7 +3048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -3000,7 +3059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -3011,7 +3070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -3022,7 +3081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -3033,7 +3092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="33" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -3044,7 +3103,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="33" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -3055,7 +3114,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="33" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -3066,7 +3125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="33" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -3077,7 +3136,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="33" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -3088,7 +3147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="33" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -3099,7 +3158,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="33" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -3110,7 +3169,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="33" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3121,7 +3180,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="33" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -3132,7 +3191,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="33" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -3143,7 +3202,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="33" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -3154,7 +3213,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="33" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3162,7 +3221,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="33" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>96</v>
       </c>
@@ -3173,7 +3232,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="33" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>96</v>
       </c>
@@ -3184,7 +3243,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="33" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>101</v>
       </c>
@@ -3195,7 +3254,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="33" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>104</v>
       </c>
@@ -3206,7 +3265,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="33" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>104</v>
       </c>
@@ -3217,7 +3276,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="33" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -3228,7 +3287,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="33" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -3239,7 +3298,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="33" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
@@ -3250,7 +3309,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="33" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>117</v>
       </c>
@@ -3261,7 +3320,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="33" customHeight="1">
       <c r="A30" s="15" t="s">
         <v>134</v>
       </c>
@@ -3272,7 +3331,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="33" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>127</v>
       </c>
@@ -3283,7 +3342,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="33" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>127</v>
       </c>
@@ -3294,7 +3353,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="33" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>130</v>
       </c>
@@ -3305,7 +3364,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="33" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>137</v>
       </c>
@@ -3316,7 +3375,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="33" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>140</v>
       </c>
@@ -3327,7 +3386,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="33" customHeight="1">
       <c r="A36" s="15" t="s">
         <v>143</v>
       </c>
@@ -3338,7 +3397,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="33" customHeight="1">
       <c r="A37" s="15" t="s">
         <v>143</v>
       </c>
@@ -3349,7 +3408,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="33" customHeight="1">
       <c r="A38" s="15" t="s">
         <v>154</v>
       </c>
@@ -3360,7 +3419,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="33" customHeight="1">
       <c r="A39" s="15" t="s">
         <v>154</v>
       </c>
@@ -3371,7 +3430,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="33" customHeight="1">
       <c r="A40" s="15" t="s">
         <v>154</v>
       </c>
@@ -3382,7 +3441,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="33" customHeight="1">
       <c r="A41" s="15" t="s">
         <v>158</v>
       </c>
@@ -3393,7 +3452,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="33" customHeight="1">
       <c r="A42" s="15" t="s">
         <v>158</v>
       </c>
@@ -3404,7 +3463,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="33" customHeight="1">
       <c r="A43" s="15" t="s">
         <v>161</v>
       </c>
@@ -3415,7 +3474,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="33" customHeight="1">
       <c r="A44" s="15" t="s">
         <v>161</v>
       </c>
@@ -3426,7 +3485,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="33" customHeight="1">
       <c r="A45" s="15" t="s">
         <v>163</v>
       </c>
@@ -3437,7 +3496,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="33" customHeight="1">
       <c r="A46" s="15" t="s">
         <v>163</v>
       </c>
@@ -3448,7 +3507,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="33" customHeight="1">
       <c r="A47" s="15" t="s">
         <v>163</v>
       </c>
@@ -3459,7 +3518,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="33" customHeight="1">
       <c r="A48" s="15" t="s">
         <v>166</v>
       </c>
@@ -3470,7 +3529,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="33" customHeight="1">
       <c r="A49" s="15" t="s">
         <v>167</v>
       </c>
@@ -3481,7 +3540,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="33" customHeight="1">
       <c r="A50" s="15" t="s">
         <v>169</v>
       </c>
@@ -3492,7 +3551,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="33" customHeight="1">
       <c r="A51" s="15" t="s">
         <v>172</v>
       </c>
@@ -3503,7 +3562,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="33" customHeight="1">
       <c r="A52" s="15" t="s">
         <v>172</v>
       </c>
@@ -3514,7 +3573,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="33" customHeight="1">
       <c r="A53" s="15" t="s">
         <v>177</v>
       </c>
@@ -3525,7 +3584,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="33" customHeight="1">
       <c r="A54" s="15" t="s">
         <v>177</v>
       </c>
@@ -3536,103 +3595,147 @@
         <v>194</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="71.45" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="33" customHeight="1">
       <c r="A57" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="33" customHeight="1">
+      <c r="A58" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="33" customHeight="1">
+      <c r="A59" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="33" customHeight="1">
+      <c r="A60" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="33" customHeight="1">
+      <c r="A61" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="33" customHeight="1">
+      <c r="A62" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="C62" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="33" customHeight="1">
       <c r="A63" s="15" t="s">
         <v>124</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="33" customHeight="1">
+      <c r="A64" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="33" customHeight="1">
+      <c r="A65" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="33" customHeight="1">
+      <c r="A66" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="33" customHeight="1">
+      <c r="A67" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3643,72 +3746,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="77.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="37.5">
       <c r="A1" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="93.75">
       <c r="A5" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="60">
       <c r="A13" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="39">
       <c r="A15" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="10" t="s">
         <v>65</v>
       </c>
@@ -3722,7 +3825,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
         <v>69</v>
       </c>
@@ -3736,7 +3839,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
         <v>73</v>
       </c>
@@ -3750,7 +3853,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="12" t="s">
         <v>75</v>
       </c>
@@ -3764,7 +3867,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="11" t="s">
         <v>78</v>
       </c>
@@ -3778,7 +3881,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
         <v>80</v>
       </c>
@@ -3792,7 +3895,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="30">
       <c r="A23" s="11" t="s">
         <v>84</v>
       </c>
@@ -3806,7 +3909,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
         <v>88</v>
       </c>
@@ -3820,7 +3923,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="43.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="46.5">
       <c r="A25" s="11" t="s">
         <v>91</v>
       </c>
@@ -3834,7 +3937,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="30">
       <c r="A26" s="11" t="s">
         <v>94</v>
       </c>
@@ -3857,31 +3960,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="82.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="39.25" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="82.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="60">
       <c r="A6" s="13">
         <v>42816</v>
       </c>
@@ -3892,7 +3995,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="13">
         <v>42814</v>
       </c>
@@ -3900,7 +4003,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" s="13">
         <v>42772</v>
       </c>
@@ -3911,7 +4014,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="13">
         <v>42772</v>
       </c>
@@ -3922,7 +4025,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="14">
         <v>42754</v>
       </c>

</xml_diff>

<commit_message>
Add index entry on Learning and Springboot, Modify java spring entries
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1050,7 +1050,7 @@
         <b/>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1061,7 +1061,7 @@
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2338,7 +2338,7 @@
         <b/>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2349,7 +2349,7 @@
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="新細明體"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2419,10 +2419,6 @@
 The main() method uses Spring Boot’s SpringApplication.run() method to launch an application. Did you notice that there wasn’t a single line of XML? No web.xml file either. This web application is 100% pure Java and you didn’t have to deal with configuring any plumbing or infrastructure.</t>
   </si>
   <si>
-    <t>驗證了猜測: dependency 在Spring boot的世界中的確是主動的, 我在項目中加入了spring-boot-starter-data-jpa, Compile 沒有問題, 但當run jar時, Spring報錯: org.springframework.beans.factory.BeanCreationException: Error creating bean with name 'org.s…
-很可能是因為Autowire不到dependency 所需的類所以報錯.</t>
-  </si>
-  <si>
     <t>More on Spring-boot IoC</t>
   </si>
   <si>
@@ -2462,28 +2458,9 @@
 </t>
   </si>
   <si>
-    <t>There is an code sample on github provided:
-https://kemitix.wordpress.com/2015/03/24/creating-an-awt-or-swing-gui-application-with-spring-boot/</t>
-  </si>
-  <si>
     <t>2 blogs talks details of springboot DI operation:
 a) Part1 on What is starters:  https://stormpath.com/blog/spring-boot-default-starters
 b) Part2 on How to DI: https://stormpath.com/blog/spring-boot-dependency-injection</t>
-  </si>
-  <si>
-    <t>Both Spring boot and Spring support non-web application, but they invoke the target classes in different way due to their design purpose:
-1. In traditional spring, we use the main method as entrance and start our logic like below:
-    public void main(...){
-        ApplicationContext context = ...
-        myBean = context.getBean(....
-2. In springboot, since the framework use the main as the configuration, the philosophy is changed upside down, everything is passive 被動地被框架調用(like the restcontroller, or scheduletask). So we can no longer add our login in main after the SpringApplication.run(...) because if we want to run any code, we need to find the suitable @annotation which can inform the framework on the time we want it to be invoked. And the simplest way is @Bean for method after the main method:
-    public void main(...){
-        SpringApplication.run(...);
-    }
-    @Bean
-    public JFrame invokeFrame(){
-        return new CustomFrame();
-    }</t>
   </si>
   <si>
     <t>Class CommandLineRunner and @Order</t>
@@ -2528,36 +2505,63 @@
     }
 }</t>
   </si>
+  <si>
+    <t>There is an code sample on github provided:
+https://kemitix.wordpress.com/2015/03/24/creating-an-awt-or-swing-gui-application-with-spring-boot/
+這個是最佳的非Web類Springboot的示例, 其中在ConfigClass中以Java-based形式定義了一個Bean, 再在Runner這個CommandLinerRunner中以Autowired的形式得到了實例, 而也正是CommnadLineRunner本身的必被執行特性使得其run methord得以執行.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>驗證了猜測: dependency 在Spring boot的世界中的確是主動的, 我在項目中加入了spring-boot-starter-data-jpa, Compile 沒有問題, 但當run jar時, Spring報錯: org.springframework.beans.factory.BeanCreationException: Error creating bean with name 'org.s…
+很可能是因為Autowire不到dependency 所需的類所以報錯.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Both Spring boot and Spring support non-web application, but they invoke the target classes in different way due to their design purpose:
+1. In traditional spring, we use the main method as entrance and start our logic like below:
+    public void main(...){
+        ApplicationContext context = ...
+        myBean = context.getBean(....
+2. In springboot, since the framework use the main as the configuration, the philosophy is changed upside down, everything is passive 被動地被框架調用(like the restcontroller, or scheduletask). So we can no longer add our login in main after the SpringApplication.run(...) because if we want to run any code, we need to find the suitable @annotation which can inform the framework on the time we want it to be invoked. And the simplest way is @Bean for method after the main method: (批: 這裡理解有誤, @Bean應其實是Java-based的Bean Clarification, 和XMLbase沒分別, 只是如果返回的是CommandLineRunner類的話, 由於CLR的特性, 即使其沒有被Autowired出去也還是會被框架調用而己, 非一個@Bean搞定, 實在不求甚解所致之誤, 但肯去判也是好樣的, 勉!)
+    public void main(...){
+        SpringApplication.run(...);
+    }
+    @Bean
+    public JFrame invokeFrame(){
+        return new CustomFrame();
+    }</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2624,7 +2628,7 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2687,7 +2691,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2733,10 +2737,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2749,7 +2756,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2823,6 +2830,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2857,6 +2865,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3032,22 +3041,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1">
+    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -3058,7 +3067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -3069,7 +3078,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3080,7 +3089,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -3091,7 +3100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -3102,7 +3111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -3113,7 +3122,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -3124,7 +3133,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -3135,7 +3144,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" customHeight="1">
+    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -3146,7 +3155,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="33" customHeight="1">
+    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -3157,7 +3166,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1">
+    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -3168,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33" customHeight="1">
+    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -3179,7 +3188,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="33" customHeight="1">
+    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -3190,7 +3199,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1">
+    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -3201,7 +3210,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="33" customHeight="1">
+    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -3212,7 +3221,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1">
+    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3223,7 +3232,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="33" customHeight="1">
+    <row r="17" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -3234,7 +3243,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="33" customHeight="1">
+    <row r="18" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -3245,7 +3254,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1">
+    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -3256,7 +3265,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="33" customHeight="1">
+    <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3264,7 +3273,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33" customHeight="1">
+    <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>96</v>
       </c>
@@ -3275,7 +3284,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33" customHeight="1">
+    <row r="22" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>96</v>
       </c>
@@ -3286,7 +3295,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="33" customHeight="1">
+    <row r="23" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>101</v>
       </c>
@@ -3297,7 +3306,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="33" customHeight="1">
+    <row r="24" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>104</v>
       </c>
@@ -3308,7 +3317,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="33" customHeight="1">
+    <row r="25" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>104</v>
       </c>
@@ -3319,7 +3328,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="33" customHeight="1">
+    <row r="26" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -3330,7 +3339,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="33" customHeight="1">
+    <row r="27" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -3341,7 +3350,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="33" customHeight="1">
+    <row r="28" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
@@ -3352,7 +3361,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="33" customHeight="1">
+    <row r="29" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>117</v>
       </c>
@@ -3363,7 +3372,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="33" customHeight="1">
+    <row r="30" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>134</v>
       </c>
@@ -3374,7 +3383,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="33" customHeight="1">
+    <row r="31" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>127</v>
       </c>
@@ -3385,7 +3394,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="33" customHeight="1">
+    <row r="32" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>127</v>
       </c>
@@ -3396,7 +3405,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="33" customHeight="1">
+    <row r="33" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>130</v>
       </c>
@@ -3407,7 +3416,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="33" customHeight="1">
+    <row r="34" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>137</v>
       </c>
@@ -3418,7 +3427,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="33" customHeight="1">
+    <row r="35" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>140</v>
       </c>
@@ -3429,7 +3438,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="33" customHeight="1">
+    <row r="36" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>143</v>
       </c>
@@ -3440,7 +3449,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="33" customHeight="1">
+    <row r="37" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>143</v>
       </c>
@@ -3451,7 +3460,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="33" customHeight="1">
+    <row r="38" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>154</v>
       </c>
@@ -3462,7 +3471,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="33" customHeight="1">
+    <row r="39" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>154</v>
       </c>
@@ -3473,7 +3482,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="33" customHeight="1">
+    <row r="40" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>154</v>
       </c>
@@ -3484,7 +3493,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="33" customHeight="1">
+    <row r="41" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
         <v>158</v>
       </c>
@@ -3495,7 +3504,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="33" customHeight="1">
+    <row r="42" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
         <v>158</v>
       </c>
@@ -3506,7 +3515,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="33" customHeight="1">
+    <row r="43" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>161</v>
       </c>
@@ -3517,7 +3526,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="33" customHeight="1">
+    <row r="44" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>161</v>
       </c>
@@ -3528,7 +3537,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="33" customHeight="1">
+    <row r="45" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="15" t="s">
         <v>163</v>
       </c>
@@ -3539,7 +3548,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="33" customHeight="1">
+    <row r="46" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>163</v>
       </c>
@@ -3550,7 +3559,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="33" customHeight="1">
+    <row r="47" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>163</v>
       </c>
@@ -3561,7 +3570,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="33" customHeight="1">
+    <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="15" t="s">
         <v>166</v>
       </c>
@@ -3572,7 +3581,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="33" customHeight="1">
+    <row r="49" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>167</v>
       </c>
@@ -3583,7 +3592,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="33" customHeight="1">
+    <row r="50" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>169</v>
       </c>
@@ -3594,7 +3603,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="33" customHeight="1">
+    <row r="51" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="15" t="s">
         <v>172</v>
       </c>
@@ -3605,7 +3614,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="33" customHeight="1">
+    <row r="52" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="s">
         <v>172</v>
       </c>
@@ -3616,7 +3625,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="33" customHeight="1">
+    <row r="53" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>177</v>
       </c>
@@ -3627,7 +3636,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="33" customHeight="1">
+    <row r="54" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="15" t="s">
         <v>177</v>
       </c>
@@ -3638,7 +3647,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="33" customHeight="1">
+    <row r="55" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>124</v>
       </c>
@@ -3649,7 +3658,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="71.45" customHeight="1">
+    <row r="56" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>124</v>
       </c>
@@ -3660,7 +3669,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="33" customHeight="1">
+    <row r="57" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>196</v>
       </c>
@@ -3671,7 +3680,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="33" customHeight="1">
+    <row r="58" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>196</v>
       </c>
@@ -3682,7 +3691,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="33" customHeight="1">
+    <row r="59" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>196</v>
       </c>
@@ -3693,7 +3702,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="33" customHeight="1">
+    <row r="60" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>201</v>
       </c>
@@ -3704,7 +3713,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="33" customHeight="1">
+    <row r="61" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>196</v>
       </c>
@@ -3715,7 +3724,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="33" customHeight="1">
+    <row r="62" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>201</v>
       </c>
@@ -3726,7 +3735,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="33" customHeight="1">
+    <row r="63" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="s">
         <v>124</v>
       </c>
@@ -3734,76 +3743,76 @@
         <v>208</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="33" customHeight="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="15" t="s">
         <v>209</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="33" customHeight="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
         <v>209</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="33" customHeight="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="B66" s="15" t="s">
-        <v>218</v>
+      <c r="B66" s="17" t="s">
+        <v>217</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="33" customHeight="1">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
         <v>209</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="33" customHeight="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="15" t="s">
         <v>209</v>
       </c>
       <c r="B68" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C68" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="C68" s="15" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="33" customHeight="1">
+    </row>
+    <row r="69" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>104</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="33" customHeight="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="15"/>
     </row>
   </sheetData>
@@ -3814,72 +3823,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="77.375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="37.5">
+    <row r="1" spans="1:1" ht="36" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75">
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="93.75">
+    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75">
+    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75">
+    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75">
+    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75">
+    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="60">
+    <row r="13" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="39">
+    <row r="15" spans="1:1" ht="53.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>65</v>
       </c>
@@ -3893,7 +3902,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>69</v>
       </c>
@@ -3907,7 +3916,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>73</v>
       </c>
@@ -3921,7 +3930,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>75</v>
       </c>
@@ -3935,7 +3944,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>78</v>
       </c>
@@ -3949,7 +3958,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>80</v>
       </c>
@@ -3963,7 +3972,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30">
+    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>84</v>
       </c>
@@ -3977,7 +3986,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>88</v>
       </c>
@@ -3991,7 +4000,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="46.5">
+    <row r="25" spans="1:4" ht="43.8" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>91</v>
       </c>
@@ -4005,7 +4014,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>94</v>
       </c>
@@ -4028,31 +4037,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="82.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.25" customWidth="1"/>
+    <col min="2" max="2" width="82.625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="39.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60">
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>42816</v>
       </c>
@@ -4063,7 +4072,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>42814</v>
       </c>
@@ -4071,7 +4080,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>42772</v>
       </c>
@@ -4082,7 +4091,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>42772</v>
       </c>
@@ -4093,7 +4102,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>42754</v>
       </c>

</xml_diff>

<commit_message>
Add java entry on JNI x JNA
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="236">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1050,7 +1050,7 @@
         <b/>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -1061,7 +1061,7 @@
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2338,7 +2338,7 @@
         <b/>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="1"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -2349,7 +2349,7 @@
       <rPr>
         <sz val="8"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -2532,36 +2532,67 @@
     }</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>JNI</t>
+  </si>
+  <si>
+    <t>JNA</t>
+  </si>
+  <si>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>REF: http://www.cnblogs.com/lanxuezaipiao/p/3635556.html
+JNI(Java Native Interface) 有过不同语言间通信经历的一般都知道，它允许Java代码和其他语言（尤其C/C++）写的代码进行交互，只要遵守调用约定即可。首先看下JNI调用C/C++的过程，注意写程序时自下而上，调用时自上而下。Java 和 C 在開發時需互相得知對方的存在。
+步骤非常的多，很麻烦，使用JNI调用.dll/.so共享库都能体会到这个痛苦的过程。如果已有一个编译好的.dll/.so文件，如果使用JNI技术调用，我们首先需要使用C语言另外写一个.dll/.so共享库，使用SUN规定的数据结构替代C语言的数据结构，调用已有的 dll/so中公布的函 数。然后再在Java中载入这个库dll/so，最后编写Java native 函数作为链接库中函数的代理。经过这些繁琐的步骤才能在Java中调用本地代码。因此，很少有Java程序员愿意编写调用dll/.so库中原生函数的java程序。这也使Java语言在客户端上乏善可陈，可以说JNI是 Java的一大弱点！</t>
+  </si>
+  <si>
+    <t>REF: http://www.cnblogs.com/lanxuezaipiao/p/3635556.html
+JNA(Java Native Access) 一个开源(Github)的Java框架，是Sun公司推出的一种调用本地方法的技术，是建立在经典的JNI基础之上的一个框架。之所以说它是JNI的替代者，是因为JNA大大简化了调用本地方法的过程，使用很方便，基本上不需要脱离Java环境就可以完成。最重要的是我们不需要重写我们的动态链接库文件，而是有直接调用的API，大大简化了我们的工作量。JNA只需要我们写Java代码而不用写JNI或本地代码。</t>
+  </si>
+  <si>
+    <t>Call Library</t>
+  </si>
+  <si>
+    <t>JNA can load system library like msvcrt.dll, or custom dll.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A complete Java - C++ connection example with mingw/g++ and JNA </t>
+  </si>
+  <si>
+    <t>ref: http://capsis.cirad.fr/capsis/documentation/java-c_connectioncompleteexample
+Super cool tutorial, I use this to finish my demo. And for code, refers to mylesieong github project: jna-demo</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="2"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2628,7 +2659,7 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -2742,8 +2773,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2756,7 +2787,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2830,7 +2861,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2865,7 +2895,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3041,22 +3070,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="33" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="68.125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.125" style="3"/>
+    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="33" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -3067,7 +3096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
@@ -3078,7 +3107,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3089,7 +3118,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -3100,7 +3129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
@@ -3111,7 +3140,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -3122,7 +3151,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -3133,7 +3162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -3144,7 +3173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="33" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
@@ -3155,7 +3184,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="33" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -3166,7 +3195,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="33" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>28</v>
       </c>
@@ -3177,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="33" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -3188,7 +3217,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="33" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -3199,7 +3228,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="33" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
@@ -3210,7 +3239,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="33" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -3221,7 +3250,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="33" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3232,7 +3261,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="33" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>46</v>
       </c>
@@ -3243,7 +3272,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="33" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -3254,7 +3283,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="33" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -3265,7 +3294,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="33" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>46</v>
       </c>
@@ -3273,7 +3302,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="33" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>96</v>
       </c>
@@ -3284,7 +3313,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="33" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>96</v>
       </c>
@@ -3295,7 +3324,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="33" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>101</v>
       </c>
@@ -3306,7 +3335,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="33" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>104</v>
       </c>
@@ -3317,7 +3346,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="33" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>104</v>
       </c>
@@ -3328,7 +3357,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="33" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>46</v>
       </c>
@@ -3339,7 +3368,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="33" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -3350,7 +3379,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="33" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>117</v>
       </c>
@@ -3361,7 +3390,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="33" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>117</v>
       </c>
@@ -3372,7 +3401,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="33" customHeight="1">
       <c r="A30" s="15" t="s">
         <v>134</v>
       </c>
@@ -3383,7 +3412,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="33" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>127</v>
       </c>
@@ -3394,7 +3423,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="33" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>127</v>
       </c>
@@ -3405,7 +3434,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="33" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>130</v>
       </c>
@@ -3416,7 +3445,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="33" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>137</v>
       </c>
@@ -3427,7 +3456,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="33" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>140</v>
       </c>
@@ -3438,7 +3467,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="33" customHeight="1">
       <c r="A36" s="15" t="s">
         <v>143</v>
       </c>
@@ -3449,7 +3478,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="33" customHeight="1">
       <c r="A37" s="15" t="s">
         <v>143</v>
       </c>
@@ -3460,7 +3489,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="33" customHeight="1">
       <c r="A38" s="15" t="s">
         <v>154</v>
       </c>
@@ -3471,7 +3500,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="33" customHeight="1">
       <c r="A39" s="15" t="s">
         <v>154</v>
       </c>
@@ -3482,7 +3511,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="33" customHeight="1">
       <c r="A40" s="15" t="s">
         <v>154</v>
       </c>
@@ -3493,7 +3522,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="33" customHeight="1">
       <c r="A41" s="15" t="s">
         <v>158</v>
       </c>
@@ -3504,7 +3533,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="33" customHeight="1">
       <c r="A42" s="15" t="s">
         <v>158</v>
       </c>
@@ -3515,7 +3544,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="33" customHeight="1">
       <c r="A43" s="15" t="s">
         <v>161</v>
       </c>
@@ -3526,7 +3555,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="33" customHeight="1">
       <c r="A44" s="15" t="s">
         <v>161</v>
       </c>
@@ -3537,7 +3566,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="33" customHeight="1">
       <c r="A45" s="15" t="s">
         <v>163</v>
       </c>
@@ -3548,7 +3577,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="33" customHeight="1">
       <c r="A46" s="15" t="s">
         <v>163</v>
       </c>
@@ -3559,7 +3588,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="33" customHeight="1">
       <c r="A47" s="15" t="s">
         <v>163</v>
       </c>
@@ -3570,7 +3599,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="33" customHeight="1">
       <c r="A48" s="15" t="s">
         <v>166</v>
       </c>
@@ -3581,7 +3610,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="33" customHeight="1">
       <c r="A49" s="15" t="s">
         <v>167</v>
       </c>
@@ -3592,7 +3621,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="33" customHeight="1">
       <c r="A50" s="15" t="s">
         <v>169</v>
       </c>
@@ -3603,7 +3632,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="33" customHeight="1">
       <c r="A51" s="15" t="s">
         <v>172</v>
       </c>
@@ -3614,7 +3643,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="33" customHeight="1">
       <c r="A52" s="15" t="s">
         <v>172</v>
       </c>
@@ -3625,7 +3654,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="33" customHeight="1">
       <c r="A53" s="15" t="s">
         <v>177</v>
       </c>
@@ -3636,7 +3665,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="33" customHeight="1">
       <c r="A54" s="15" t="s">
         <v>177</v>
       </c>
@@ -3647,7 +3676,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>124</v>
       </c>
@@ -3658,7 +3687,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="71.45" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>124</v>
       </c>
@@ -3669,7 +3698,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="33" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>196</v>
       </c>
@@ -3680,7 +3709,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="33" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>196</v>
       </c>
@@ -3691,7 +3720,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="33" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>196</v>
       </c>
@@ -3702,7 +3731,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="33" customHeight="1">
       <c r="A60" s="15" t="s">
         <v>201</v>
       </c>
@@ -3713,7 +3742,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="33" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>196</v>
       </c>
@@ -3724,7 +3753,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="33" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>201</v>
       </c>
@@ -3735,7 +3764,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="33" customHeight="1">
       <c r="A63" s="15" t="s">
         <v>124</v>
       </c>
@@ -3746,7 +3775,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="33" customHeight="1">
       <c r="A64" s="15" t="s">
         <v>209</v>
       </c>
@@ -3757,7 +3786,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="33" customHeight="1">
       <c r="A65" s="15" t="s">
         <v>209</v>
       </c>
@@ -3768,7 +3797,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="33" customHeight="1">
       <c r="A66" s="15" t="s">
         <v>209</v>
       </c>
@@ -3779,7 +3808,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="33" customHeight="1">
       <c r="A67" s="15" t="s">
         <v>209</v>
       </c>
@@ -3790,7 +3819,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="33" customHeight="1">
       <c r="A68" s="15" t="s">
         <v>209</v>
       </c>
@@ -3801,7 +3830,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="33" customHeight="1">
       <c r="A69" s="15" t="s">
         <v>104</v>
       </c>
@@ -3812,8 +3841,49 @@
         <v>222</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="15"/>
+    <row r="70" spans="1:3" ht="33" customHeight="1">
+      <c r="A70" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="33" customHeight="1">
+      <c r="A71" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="33" customHeight="1">
+      <c r="A72" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="33" customHeight="1">
+      <c r="A73" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>235</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3823,72 +3893,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="77.375" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="77.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="36" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="37.5">
       <c r="A1" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="90" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="93.75">
       <c r="A5" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="60">
       <c r="A13" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="39">
       <c r="A15" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="10" t="s">
         <v>65</v>
       </c>
@@ -3902,7 +3972,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
         <v>69</v>
       </c>
@@ -3916,7 +3986,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
         <v>73</v>
       </c>
@@ -3930,7 +4000,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="12" t="s">
         <v>75</v>
       </c>
@@ -3944,7 +4014,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="11" t="s">
         <v>78</v>
       </c>
@@ -3958,7 +4028,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
         <v>80</v>
       </c>
@@ -3972,7 +4042,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="30">
       <c r="A23" s="11" t="s">
         <v>84</v>
       </c>
@@ -3986,7 +4056,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
         <v>88</v>
       </c>
@@ -4000,7 +4070,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="43.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="46.5">
       <c r="A25" s="11" t="s">
         <v>91</v>
       </c>
@@ -4014,7 +4084,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="30">
       <c r="A26" s="11" t="s">
         <v>94</v>
       </c>
@@ -4037,31 +4107,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.25" customWidth="1"/>
-    <col min="2" max="2" width="82.625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="39.25" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="82.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="60">
       <c r="A6" s="13">
         <v>42816</v>
       </c>
@@ -4072,7 +4142,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="13">
         <v>42814</v>
       </c>
@@ -4080,7 +4150,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" s="13">
         <v>42772</v>
       </c>
@@ -4091,7 +4161,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" s="13">
         <v>42772</v>
       </c>
@@ -4102,7 +4172,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="14">
         <v>42754</v>
       </c>

</xml_diff>

<commit_message>
Add bitwise operand intro
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="9720" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="239">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -2562,6 +2562,19 @@
   <si>
     <t>ref: http://capsis.cirad.fr/capsis/documentation/java-c_connectioncompleteexample
 Super cool tutorial, I use this to finish my demo. And for code, refers to mylesieong github project: jna-demo</t>
+  </si>
+  <si>
+    <t># Operand</t>
+  </si>
+  <si>
+    <t>## Bitwise Operand</t>
+  </si>
+  <si>
+    <t>* &amp; is  bitwise AND
+* | is bitwise OR
+* ^ -is bitwise XOR, that return if not same of a and b at the same bit 位 
+* &gt;&gt; is bitwise shift to right
+* &gt;&gt;&gt;  是 &gt;&gt; 但補零</t>
   </si>
 </sst>
 </file>
@@ -3071,10 +3084,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="C67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
@@ -3883,6 +3896,17 @@
       </c>
       <c r="C73" s="15" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="33" customHeight="1">
+      <c r="A74" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry on jvm and java covert
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -11,7 +11,11 @@
     <sheet name="jdbc  connection properties" sheetId="2" r:id="rId2"/>
     <sheet name="the source" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="A">[1]options!$B$2:$B$4</definedName>
     <definedName name="TagOptions">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="246">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -2575,6 +2579,44 @@
 * ^ -is bitwise XOR, that return if not same of a and b at the same bit 位 
 * &gt;&gt; is bitwise shift to right
 * &gt;&gt;&gt;  是 &gt;&gt; 但補零</t>
+  </si>
+  <si>
+    <t># JVM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* JVM is java.exe
+* In JVM, new objects are create and placed in HEAP (Garbage Collector works toward HEAP)
+* In JVM, call method state are stored in STACK (so that we have printStackTrace)
+* Threads have their own call STACK (so that they can run independently)
+* when run JVM (java.exe), OS will assign fixed available memory (min + max). What we see in Windows Task Manager is x within period(min, max).
+* Set Heap size of JVM
+` $ java -Xms1024m ... //set min available memory to 1024 MB`  
+` $ java -Xmx1800m ... //set max available memory to 1800 MB` </t>
+  </si>
+  <si>
+    <t>## Intro to JVM</t>
+  </si>
+  <si>
+    <t>## Classpath &amp; Bootclasspath</t>
+  </si>
+  <si>
+    <t>## JVM Option Help</t>
+  </si>
+  <si>
+    <t>`java -X`</t>
+  </si>
+  <si>
+    <t>### Classapth (java -cp)
+* 2 kinds of classpath can be assgined to JVM:
+    * A ; seperated list of directories
+    * A jar archives
+* JVM will use the first found X.class in the classpath, with this feature, we can stub any class to our application. (but not apply to core class in rt.jar)
+### Bootclasspath (java -Xbootclasspath)
+* Boot Classpath is default as your $JRE_HOME/lib, that almost all jdk core classes are included.
+* It need not to be defined whenever we run JVM and its loaded by default
+* We can override it with -Xbootclasspath, -Xbootclasspath/a, -Xbootclasspath/p
+* With overriding the bootclasspath, we can stub the core classes 
+_refs to my github/stub-a-library-demo for detail_</t>
   </si>
 </sst>
 </file>
@@ -2797,6 +2839,43 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="index"/>
+      <sheetName val="options"/>
+      <sheetName val="AS400 Version"/>
+      <sheetName val="Apache Overview"/>
+      <sheetName val="Apache Details"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>#concept</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>#resource</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>#fact</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3084,10 +3163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
@@ -3907,6 +3986,39 @@
       </c>
       <c r="C74" s="15" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="33" customHeight="1">
+      <c r="A75" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="33" customHeight="1">
+      <c r="A76" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="33" customHeight="1">
+      <c r="A77" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry about Basic IO introduction
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="262">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -127,14 +127,6 @@
 $mvn eclipse:eclipse -Dwtpversion=2.0
 2. Imports it into Eclipse IDE
 File -&gt; Import… -&gt; General -&gt; Existing Projects into workspace</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>$ mvn archetype:generate 
-        -DgroupId={project-packaging} 
-        -DartifactId={project-name} 
-        -DarchetypeArtifactId=maven-archetype-webapp 
-        -DinteractiveMode=false</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -2652,6 +2644,125 @@
       </rPr>
       <t>minimize the need to change the well-tested code</t>
     </r>
+  </si>
+  <si>
+    <t># Encoding</t>
+  </si>
+  <si>
+    <t>## Communicate between system in different charset</t>
+  </si>
+  <si>
+    <t># Runtime.exec</t>
+  </si>
+  <si>
+    <t>## Runtime.exec()</t>
+  </si>
+  <si>
+    <t># How to run a command from java
+Runtime rt = Runtime.getRuntime();
+Process p = rt.exec("javac");
+# Process.waitFor() vs Process.exitVal()
+# Why Process.waitFor() hangs
+ref: http://www.javaworld.com/article/2071275/core-java/when-runtime-exec---won-t.html
+ref: https://stackoverflow.com/questions/5483830/process-waitfor-never-returns</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Code Snippet
+Say system A use "ISO1234" and system B use "UTF8", given the scenario that we read data from system A on system B with the following:
+```java
+String sA = req.getParameter("Prop_of_A");
+String sB = new String( sA.getBytes("ISO1234"), "UTF8");
+```
+# Must-know Concept
+* Java String class does not take the byte as its core, it take the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>char</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> group itself. So that's why charset is the property that we inject in String: getBytes() method
+* For a smaller charset system, the data through this system might has a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>resolution-lost.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> In this way, better transfer data in byte form (the most native form) so to prevent the lost.</t>
+    </r>
+  </si>
+  <si>
+    <t>$ mvn archetype:generate 
+        -DgroupId={project-packaging} 
+        -DartifactId={project-name} 
+        -DarchetypeArtifactId=maven-archetype-webapp 
+        -DinteractiveMode=false</t>
+  </si>
+  <si>
+    <t>Basic IO</t>
+  </si>
+  <si>
+    <t>Stream Wrappers</t>
+  </si>
+  <si>
+    <t>Atomic Stream and Writer/Reader</t>
+  </si>
+  <si>
+    <t>Writer/Reader Wrappers</t>
+  </si>
+  <si>
+    <t>To add feature to the Writer/ Reader, java provides classes as wrapper on top of them, they are:
+* BufferedWriter 
+* PrintWriter
+* BufferedReader
+* Scanner</t>
+  </si>
+  <si>
+    <t>To add feature to the Stream, java provides classes as wrapper on top of Input/Output stream, they are:
+* BufferedInputStream (Native API called when buffer empty)
+* Scanner 
+* BufferedOutputStream (Native API called when buffer full)</t>
+  </si>
+  <si>
+    <t>Stream and Writer/Reader is the 2 pillars that support the whole Java IO. 
+## Stream Definition
+Stream abstract the concept of a information stream from data source to program. The famous, symbolic and atomic stream are:
+* FileInputStream
+* FileOutputStream
+## Writer/ Reader Definition
+Writer/ Reader abstract the concept of a data receiver/ sender at the program end. All of them hold a stream as their porperty. Famous classes are:
+* FileReader
+* FileWriter</t>
   </si>
 </sst>
 </file>
@@ -3206,23 +3317,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="68.140625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -3233,7 +3344,7 @@
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -3244,18 +3355,18 @@
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>133</v>
+      <c r="C3" s="15" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -3266,7 +3377,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -3277,7 +3388,7 @@
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -3288,18 +3399,18 @@
     </row>
     <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
+      <c r="C7" s="15" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -3310,29 +3421,29 @@
     </row>
     <row r="9" spans="1:3" ht="33" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="33" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="33" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -3346,733 +3457,788 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="33" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="33" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="33" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="33" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="33" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="33" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="33" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="33" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="33" customHeight="1">
       <c r="A21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="33" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="33" customHeight="1">
       <c r="A23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="33" customHeight="1">
       <c r="A24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="33" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>107</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="33" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="33" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>115</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="33" customHeight="1">
       <c r="A28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="33" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="33" customHeight="1">
       <c r="A30" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="C30" s="15" t="s">
         <v>135</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="33" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="33" customHeight="1">
       <c r="A32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="33" customHeight="1">
       <c r="A33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="33" customHeight="1">
       <c r="A34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="33" customHeight="1">
       <c r="A35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="33" customHeight="1">
       <c r="A36" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="C36" s="15" t="s">
         <v>144</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="33" customHeight="1">
       <c r="A37" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>146</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="33" customHeight="1">
       <c r="A38" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="B38" s="15" t="s">
-        <v>155</v>
-      </c>
       <c r="C38" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="33" customHeight="1">
       <c r="A39" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="33" customHeight="1">
       <c r="A40" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="33" customHeight="1">
       <c r="A41" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B41" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>159</v>
-      </c>
       <c r="C41" s="15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="33" customHeight="1">
       <c r="A42" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="33" customHeight="1">
       <c r="A43" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="33" customHeight="1">
       <c r="A44" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>162</v>
-      </c>
       <c r="C44" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="33" customHeight="1">
       <c r="A45" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>164</v>
-      </c>
       <c r="C45" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="33" customHeight="1">
       <c r="A46" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="33" customHeight="1">
       <c r="A47" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="33" customHeight="1">
       <c r="A48" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="33" customHeight="1">
       <c r="A49" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="B49" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="B49" s="15" t="s">
-        <v>168</v>
-      </c>
       <c r="C49" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="33" customHeight="1">
       <c r="A50" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>170</v>
-      </c>
       <c r="C50" s="15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="33" customHeight="1">
       <c r="A51" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="B51" s="15" t="s">
-        <v>173</v>
-      </c>
       <c r="C51" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="33" customHeight="1">
       <c r="A52" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="33" customHeight="1">
       <c r="A53" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="33" customHeight="1">
       <c r="A54" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B54" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="B54" s="15" t="s">
-        <v>178</v>
-      </c>
       <c r="C54" s="15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="33" customHeight="1">
       <c r="A55" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="71.45" customHeight="1">
       <c r="A56" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="33" customHeight="1">
       <c r="A57" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>197</v>
-      </c>
       <c r="C57" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="33" customHeight="1">
       <c r="A58" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="33" customHeight="1">
       <c r="A59" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="33" customHeight="1">
       <c r="A60" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="B60" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="B60" s="15" t="s">
-        <v>202</v>
-      </c>
       <c r="C60" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="33" customHeight="1">
       <c r="A61" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="33" customHeight="1">
       <c r="A62" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C62" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="33" customHeight="1">
       <c r="A63" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="33" customHeight="1">
       <c r="A64" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="33" customHeight="1">
       <c r="A65" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="33" customHeight="1">
       <c r="A66" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="33" customHeight="1">
       <c r="A67" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="33" customHeight="1">
       <c r="A68" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="33" customHeight="1">
       <c r="A69" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B69" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C69" s="15" t="s">
         <v>221</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="33" customHeight="1">
       <c r="A70" s="15" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B70" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C70" s="15" t="s">
         <v>229</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="33" customHeight="1">
       <c r="A71" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="B71" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="B71" s="15" t="s">
-        <v>229</v>
-      </c>
       <c r="C71" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="33" customHeight="1">
       <c r="A72" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B72" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="C72" s="15" t="s">
         <v>232</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="33" customHeight="1">
       <c r="A73" s="15" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B73" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C73" s="15" t="s">
         <v>234</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="33" customHeight="1">
       <c r="A74" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B74" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="C74" s="15" t="s">
         <v>237</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="33" customHeight="1">
       <c r="A75" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C75" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="B75" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="33" customHeight="1">
       <c r="A76" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B76" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="C76" s="15" t="s">
         <v>243</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="33" customHeight="1">
       <c r="A77" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="33" customHeight="1">
       <c r="A78" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="B78" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="C78" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="C78" s="15" t="s">
+    </row>
+    <row r="79" spans="1:3" ht="33" customHeight="1">
+      <c r="A79" s="15" t="s">
         <v>248</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="33" customHeight="1">
+      <c r="A80" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C80" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="33" customHeight="1">
+      <c r="A81" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="57">
+      <c r="A82" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="57">
+      <c r="A83" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -4100,190 +4266,190 @@
   <sheetData>
     <row r="1" spans="1:1" ht="37.5">
       <c r="A1" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="93.75">
       <c r="A5" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="60">
       <c r="A13" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="39">
       <c r="A15" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>67</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30">
       <c r="A23" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>86</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="C24" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="46.5">
       <c r="A25" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C25" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
       <c r="A26" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -4313,12 +4479,12 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60">
@@ -4326,10 +4492,10 @@
         <v>42816</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4337,7 +4503,7 @@
         <v>42814</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45">
@@ -4345,10 +4511,10 @@
         <v>42772</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4356,10 +4522,10 @@
         <v>42772</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45">
@@ -4367,7 +4533,7 @@
         <v>42754</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>

<commit_message>
Add java entry on java io and nio
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -15,7 +15,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="A">[1]options!$B$2:$B$4</definedName>
+    <definedName name="A">#REF!</definedName>
     <definedName name="TagOptions">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="271">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -2757,19 +2757,174 @@
     <t>Stream and Writer/Reader is the 2 pillars that support the whole Java IO. 
 ## Stream Definition
 Stream abstract the concept of a information stream from data source to program. The famous, symbolic and atomic stream are:
-* FileInputStream
-* FileOutputStream
+* File(In/Out)putStream
+* Data(In/Out)putStream
+* Object(In/Out)Stream
 ## Writer/ Reader Definition
 Writer/ Reader abstract the concept of a data receiver/ sender at the program end. All of them hold a stream as their porperty. Famous classes are:
 * FileReader
-* FileWriter</t>
+* FileWriter
+## Understanding all this shit
+Its doom to abstract the concept of Java IO from program perspective which is too complicated. It is easier if we try to understand it from the Object-Oriented Abstraction Point of View. In this way, Input/Output Stream define most of the behavior in JavaIO and that's it.</t>
+  </si>
+  <si>
+    <t>Why NIO</t>
+  </si>
+  <si>
+    <t>NIO</t>
+  </si>
+  <si>
+    <t>Bridge between io &amp; nio</t>
+  </si>
+  <si>
+    <r>
+      <t>import java.io.File;
+import java.nio.file.Path;
+…
+File file = new File();
+Path path = file.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>toPath</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>();  // from io to nio
+…
+Path path = new Path();
+File file = path.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>toFile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>();  // from nio to io</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t># When
+The NIO (New IO) is introduced to Java since 7. 
+# Why 
+Old java.io.File class had several drawbacks.
+* No specify error msg from file delete failure
+* Rename feature not stable
+* No support for symbolic links and cannot recognize it.
+* Not enough support for metadata
+* Many of the File methods didn't scale (scalable)
+# The Implementation
+Java nio was built base on a total different perspective than java io</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(io use File abstraction but nio use Path abstraction)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. But both provide similar functionality. To map them by functionality, reference to the legacy-mapping part in java official tutorial.</t>
+    </r>
+  </si>
+  <si>
+    <t>Basic Operation (1)</t>
+  </si>
+  <si>
+    <t>Basic Operation (2)</t>
+  </si>
+  <si>
+    <t># Allocate Resource
+Path p = Paths.get("/etc/abc.conf" );
+# File/ directory manipulation
+Files.exists(p);
+Files.isReadable(p);
+Files.isSameFile(p1, p2);
+Files.delete(p);  //different exception will be thrown, awesome
+Files.copy(p1, p2, StandardCopyOption.REPLACE_EXISTING);
+Files.move(p1, p2, StandardCopyOption.REPLACE_EXISTING);
+Files.createFile(p);</t>
+  </si>
+  <si>
+    <t># Read for small file
+Path file = ...;
+byte[] fileArray;
+fileArray = Files.readAllBytes(file);
+# Write for small file
+Path file = ...;
+byte[] buf = ...;
+Files.write(file, buf);
+# Read for big file (use Reader)
+Charset charset = Charset.forName("US-ASCII");
+BufferedReader reader = Files.newBufferedReader(path, charset);
+while ((line = reader.readLine()) != null) {
+        System.out.println(line);
+}
+# Read for big file (use Stream)
+InputStream in = Files.newInputStream(file);
+BufferedReader reader = new BufferedReader(new InputStreamReader(in));
+while ((line = reader.readLine()) != null) {
+        System.out.println(line);
+}
+# Write for big file (use Writer)
+Charset charset = Charset.forName("US-ASCII");
+String s = ...;
+try (BufferedWriter writer = Files.newBufferedWriter(file, charset)) {
+    writer.write(s, 0, s.length());
+} catch (IOException x) {
+    System.err.format("IOException: %s%n", x);
+}
+# Write for big file (use Stream to adopt old io)
+    try (OutputStream out = new BufferedOutputStream(
+      Files.newOutputStream(p, CREATE, APPEND))) {
+      out.write(data, 0, data.length);
+    } catch (IOException x) {
+      System.err.println(x);
+    }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2869,6 +3024,13 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3000,33 +3162,27 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="index"/>
-      <sheetName val="options"/>
-      <sheetName val="AS400 Version"/>
-      <sheetName val="Apache Overview"/>
-      <sheetName val="Apache Details"/>
+      <sheetName val="g2k"/>
+      <sheetName val="pf meaning"/>
+      <sheetName val="imodule"/>
+      <sheetName val="CFSORC"/>
+      <sheetName val="icbs_utility"/>
+      <sheetName val="in-house"/>
+      <sheetName val="SRP"/>
+      <sheetName val="as400 cust-option"/>
+      <sheetName val="doom_code"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>#concept</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>#resource</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>#fact</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3317,10 +3473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
@@ -4208,7 +4364,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="33" customHeight="1">
+    <row r="81" spans="1:3" ht="180.75">
       <c r="A81" s="15" t="s">
         <v>255</v>
       </c>
@@ -4239,6 +4395,50 @@
       </c>
       <c r="C83" s="15" t="s">
         <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="147">
+      <c r="A84" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="90.75">
+      <c r="A85" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C85" s="15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="113.25">
+      <c r="A86" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="174" customHeight="1">
+      <c r="A87" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry about RTFM concurrecy
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -11,9 +11,6 @@
     <sheet name="jdbc  connection properties" sheetId="2" r:id="rId2"/>
     <sheet name="the source" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="A">#REF!</definedName>
     <definedName name="TagOptions">#REF!</definedName>
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="278">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -2729,18 +2726,6 @@
         -DinteractiveMode=false</t>
   </si>
   <si>
-    <t>Basic IO</t>
-  </si>
-  <si>
-    <t>Stream Wrappers</t>
-  </si>
-  <si>
-    <t>Atomic Stream and Writer/Reader</t>
-  </si>
-  <si>
-    <t>Writer/Reader Wrappers</t>
-  </si>
-  <si>
     <t>To add feature to the Writer/ Reader, java provides classes as wrapper on top of them, they are:
 * BufferedWriter 
 * PrintWriter
@@ -2766,15 +2751,6 @@
 * FileWriter
 ## Understanding all this shit
 Its doom to abstract the concept of Java IO from program perspective which is too complicated. It is easier if we try to understand it from the Object-Oriented Abstraction Point of View. In this way, Input/Output Stream define most of the behavior in JavaIO and that's it.</t>
-  </si>
-  <si>
-    <t>Why NIO</t>
-  </si>
-  <si>
-    <t>NIO</t>
-  </si>
-  <si>
-    <t>Bridge between io &amp; nio</t>
   </si>
   <si>
     <r>
@@ -2865,12 +2841,6 @@
     </r>
   </si>
   <si>
-    <t>Basic Operation (1)</t>
-  </si>
-  <si>
-    <t>Basic Operation (2)</t>
-  </si>
-  <si>
     <t># Allocate Resource
 Path p = Paths.get("/etc/abc.conf" );
 # File/ directory manipulation
@@ -2918,6 +2888,203 @@
     } catch (IOException x) {
       System.err.println(x);
     }</t>
+  </si>
+  <si>
+    <t>RTFM</t>
+  </si>
+  <si>
+    <t>Basic IO: Atomic Stream and Writer/Reader</t>
+  </si>
+  <si>
+    <t>Basic IO: Stream Wrappers</t>
+  </si>
+  <si>
+    <t>Basic IO: Writer/Reader Wrappers</t>
+  </si>
+  <si>
+    <t>NIO: Why NIO</t>
+  </si>
+  <si>
+    <t>NIO: Bridge between io &amp; nio</t>
+  </si>
+  <si>
+    <t>NIO: Basic Operation (1)</t>
+  </si>
+  <si>
+    <t>NIO: Basic Operation (2)</t>
+  </si>
+  <si>
+    <t>Concurrency: Basic Idea</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Package location
+java.util.concurrent
+# Basic Object
+Thread and Process
+# Processes
+A process has a self-contained execution environment. A process generally has a complete, private set of basic run-time resources; in particular, each process has its own memory space. Processes are often seen as synonymous with programs or applications. However, what the user sees as a single application may in fact be a set of cooperating processes.
+# Threads
+Threads are sometimes called </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>lightweight processes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Both processes and threads provide an execution environment, but creating a new thread requires fewer resources than creating a new process. Threads exist within a process — every process has at least one. Threads</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> share</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the process's resources, including memory and open files.</t>
+    </r>
+  </si>
+  <si>
+    <t>Concurrency: Runnable and Thread</t>
+  </si>
+  <si>
+    <t># Create Runnable
+public class HelloRunnable implements Runnable {
+    public void run() {
+        System.out.println("Hello from a thread!");
+    }
+    public static void main(String args[]) {
+        (new Thread(new HelloRunnable())).start();
+    }
+}
+# Create Thread
+public class HelloThread extends Thread {
+    public void run() {
+        System.out.println("Hello from a thread!");
+    }
+    public static void main(String args[]) {
+        (new HelloThread()).start();
+    }
+}
+# Which one is better
+Suggest Runnable because the class can then still heritage other class</t>
+  </si>
+  <si>
+    <t>Concurrency: Intrrupt</t>
+  </si>
+  <si>
+    <t>Concurrency: Get the current thread/ API power</t>
+  </si>
+  <si>
+    <t>In any java thread, use Thread class's static method to get Thread API power such as:
+* Thread.sleep()
+* Thread.interrupted()
+* Thread.currentThread()</t>
+  </si>
+  <si>
+    <t>Threads can be interrupt by a brunch of reasons. When it is interrupted, Java Runtime will invoke thread.interrupt() method, then the object's interrupted property is set to be true. User can also throws their InterruptedException. 
+# Example of main java thread interrupting a thread created by itself when new thread makes main thread wait too long
+public class SimpleThreads {
+    // Display a message, preceded by
+    // the name of the current thread
+    static void threadMessage(String message) {
+        String threadName =
+            Thread.currentThread().getName();
+        System.out.format("%s: %s%n",
+                          threadName,
+                          message);
+    }
+    private static class MessageLoop
+        implements Runnable {
+        public void run() {
+            String importantInfo[] = {
+                "Mares eat oats",
+                "Does eat oats",
+                "Little lambs eat ivy",
+                "A kid will eat ivy too"
+            };
+            try {
+                for (int i = 0;
+                     i &lt; importantInfo.length;
+                     i++) {
+                    // Pause for 4 seconds
+                    Thread.sleep(4000);
+                    // Print a message
+                    threadMessage(importantInfo[i]);
+                }
+            } catch (InterruptedException e) {
+                threadMessage("I wasn't done!");
+            }
+        }
+    }
+    public static void main(String args[])
+        throws InterruptedException {
+        // Delay, in milliseconds before
+        // we interrupt MessageLoop
+        // thread (default one hour).
+        long patience = 1000 * 60 * 60;
+        // If command line argument
+        // present, gives patience
+        // in seconds.
+        if (args.length &gt; 0) {
+            try {
+                patience = Long.parseLong(args[0]) * 1000;
+            } catch (NumberFormatException e) {
+                System.err.println("Argument must be an integer.");
+                System.exit(1);
+            }
+        }
+        threadMessage("Starting MessageLoop thread");
+        long startTime = System.currentTimeMillis();
+        Thread t = new Thread(new MessageLoop());
+        t.start();
+        threadMessage("Waiting for MessageLoop thread to finish");
+        // loop until MessageLoop
+        // thread exits
+        while (t.isAlive()) {
+            threadMessage("Still waiting...");
+            // Wait maximum of 1 second
+            // for MessageLoop thread
+            // to finish.
+            t.join(1000);
+            if (((System.currentTimeMillis() - startTime) &gt; patience)
+                  &amp;&amp; t.isAlive()) {
+                threadMessage("Tired of waiting!");
+                t.interrupt();
+                // Shouldn't be long now
+                // -- wait indefinitely
+                t.join();
+            }
+        }
+        threadMessage("Finally!");
+    }
+}</t>
   </si>
 </sst>
 </file>
@@ -3155,37 +3322,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="index"/>
-      <sheetName val="g2k"/>
-      <sheetName val="pf meaning"/>
-      <sheetName val="imodule"/>
-      <sheetName val="CFSORC"/>
-      <sheetName val="icbs_utility"/>
-      <sheetName val="in-house"/>
-      <sheetName val="SRP"/>
-      <sheetName val="as400 cust-option"/>
-      <sheetName val="doom_code"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3473,10 +3609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
@@ -4366,79 +4502,123 @@
     </row>
     <row r="81" spans="1:3" ht="180.75">
       <c r="A81" s="15" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="B81" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C81" s="15" t="s">
         <v>257</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="57">
       <c r="A82" s="15" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="B82" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C82" s="15" t="s">
         <v>256</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="57">
       <c r="A83" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="C83" s="15" t="s">
         <v>255</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>258</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="147">
       <c r="A84" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="90.75">
       <c r="A85" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="113.25">
       <c r="A86" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="174" customHeight="1">
       <c r="A87" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C87" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="158.25">
+      <c r="A88" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B88" s="15" t="s">
         <v>270</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="33" customHeight="1">
+      <c r="A89" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="33" customHeight="1">
+      <c r="A90" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="33" customHeight="1">
+      <c r="A91" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B91" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry on RTFM: Concurrency Sync and Volatile
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="290">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -3085,6 +3085,150 @@
         threadMessage("Finally!");
     }
 }</t>
+  </si>
+  <si>
+    <t>Java Language and Virtual Machine Specifications</t>
+  </si>
+  <si>
+    <t># The full specification of Java SE: https://docs.oracle.com/javase/specs/index.html
+For the Java SE 8 Language spec, 788 pages in PDF
+For the Java SE 8 VM Spec, 604 pages in PDF</t>
+  </si>
+  <si>
+    <t>Threads communicate primarily by sharing access to fields and the objects reference fields refer to. This form of communication is extremely efficient, but makes two kinds of errors possible: 
+* Thread interference 
+2 multi-step operation on the same object, 1 of them will lost effectiveness
+* Memory consistency errors
+E.g. 2 threads operate on 1 object, when 1 thread ask for object's latest status, the status enquiry method might "HAPPENS-BEFORE" the finish of the in-process object change. That changes to the state of the object are not guaranteed to be visible to all threads</t>
+  </si>
+  <si>
+    <t>To make a method synchronized, simply add the synchronized keyword to its declaration:
+public class SynchronizedCounter {
+    private int c = 0;
+    public synchronized void increment() {        c++;    }
+    public synchronized void decrement() {        c--;    }
+    public synchronized int value() {        return c;}
+}
+If count is an instance of SynchronizedCounter, then making these methods synchronized has two effects:
+1. it is not possible for two invocations of synchronized methods on the same object to interleave. When one thread is executing a synchronized method for an object, all other threads that invoke synchronized methods for the same object block (suspend execution) until the first thread is done with the object.
+2. when a synchronized method exits, it automatically establishes a happens-before relationship with any subsequent invocation of a synchronized method for the same object. This guarantees that changes to the state of the object are visible to all threads.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concurrency: Threads communicate Problem </t>
+  </si>
+  <si>
+    <t>Concurrency: Sync Method Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concurrency: Synchronization </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2 types of Synchronization: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>synchronized methods</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>synchronized statements</t>
+    </r>
+  </si>
+  <si>
+    <t># Example 1
+public void addName(String name) {
+    synchronized(this) {
+        lastName = name;
+        nameCount++;
+    }
+    nameList.add(name);
+}
+# Example 2
+public class MsLunch {
+    private long c1 = 0;
+    private long c2 = 0;
+    private Object lock1 = new Object();
+    private Object lock2 = new Object();
+    public void inc1() {
+        synchronized(lock1) {
+            c1++;
+        }
+    }
+    public void inc2() {
+        synchronized(lock2) {
+            c2++;
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>Concurrency: Sync Statement Example</t>
+  </si>
+  <si>
+    <t>Concurrency: Make object Atomic with Volatile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p.s Though Volatile can effectively stop Thread Interference, it sill cannot eliminate Memory Consistency Errors.
+# Exampele
+public class VolatileTest {
+    private static final Logger LOGGER = MyLoggerFactory.getSimplestLogger();
+    private static volatile int MY_INT = 0;
+    public static void main(String[] args) {
+        new ChangeListener().start();
+        new ChangeMaker().start();
+    }
+    static class ChangeListener extends Thread {
+        @Override
+        public void run() {
+            int local_value = MY_INT;
+            while ( local_value &lt; 5){
+                if( local_value!= MY_INT){
+                    LOGGER.log(Level.INFO,"Got Change for MY_INT : {0}", MY_INT);
+                     local_value= MY_INT;
+                }
+            }
+        }
+    }
+    static class ChangeMaker extends Thread{
+        @Override
+        public void run() {
+            int local_value = MY_INT;
+            while (MY_INT &lt;5){
+                LOGGER.log(Level.INFO, "Incrementing MY_INT to {0}", local_value+1);
+                MY_INT = ++local_value;
+                try {
+                    Thread.sleep(500);
+                } catch (InterruptedException e) { e.printStackTrace(); }
+            }
+        }
+    }
+}
+</t>
   </si>
 </sst>
 </file>
@@ -3609,10 +3753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
@@ -4619,6 +4763,72 @@
       </c>
       <c r="C91" s="15" t="s">
         <v>276</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="33" customHeight="1">
+      <c r="A92" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B92" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="C92" s="15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="64.5" customHeight="1">
+      <c r="A93" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="33" customHeight="1">
+      <c r="A94" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="33" customHeight="1">
+      <c r="A95" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B95" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="33" customHeight="1">
+      <c r="A96" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="C96" s="15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="33" customHeight="1">
+      <c r="A97" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry on RTFM: Concurrency> Locks and Solution
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="298">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -100,15 +100,6 @@
   </si>
   <si>
     <t>Code Ref</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>JButton testButton = new JButton("Test Button");
-testButton.addActionListener(new ActionListener(){
-    @Override public void actionPerformed(ActionEvent ae){
-        System.out.println("Click Detected by Anon Class");
-    }
-});</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -3229,6 +3220,338 @@
     }
 }
 </t>
+  </si>
+  <si>
+    <t>JButton testButton = new JButton("Test Button");
+testButton.addActionListener(new ActionListener(){
+    @Override public void actionPerformed(ActionEvent ae){
+        System.out.println("Click Detected by Anon Class");
+    }
+});</t>
+  </si>
+  <si>
+    <t>Concurrency: Liveness and Problems (2)</t>
+  </si>
+  <si>
+    <t>Concurrency: Liveness and Problems (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here is an example to aviod deadlocks, strarvation and livelocks using Object.notify() method. The example "Producer" x "Consumer" x "Product"
+public class Drop {
+    // Message sent from producer
+    // to consumer.
+    private String message;
+    // True if consumer should wait
+    // for producer to send message,
+    // false if producer should wait for
+    // consumer to retrieve message.
+    private boolean empty = true;
+    public synchronized String take() {
+        // Wait until message is
+        // available.
+        while (empty) {
+            try {
+                wait();
+            } catch (InterruptedException e) {}
+        }
+        // Toggle status.
+        empty = true;
+        // Notify producer that
+        // status has changed.
+        notifyAll();
+        return message;
+    }
+    public synchronized void put(String message) {
+        // Wait until message has
+        // been retrieved.
+        while (!empty) {
+            try { 
+                wait();
+            } catch (InterruptedException e) {}
+        }
+        // Toggle status.
+        empty = false;
+        // Store message.
+        this.message = message;
+        // Notify consumer that status
+        // has changed.
+        notifyAll();
+    }
+}
+import java.util.Random;
+public class Producer implements Runnable {
+    private Drop drop;
+    public Producer(Drop drop) {
+        this.drop = drop;
+    }
+    public void run() {
+        String importantInfo[] = {
+            "Mares eat oats",
+            "Does eat oats",
+            "Little lambs eat ivy",
+            "A kid will eat ivy too"
+        };
+        Random random = new Random();
+        for (int i = 0;
+             i &lt; importantInfo.length;
+             i++) {
+            drop.put(importantInfo[i]);
+            try {
+                Thread.sleep(random.nextInt(5000));
+            } catch (InterruptedException e) {}
+        }
+        drop.put("DONE");
+    }
+}
+import java.util.Random;
+public class Consumer implements Runnable {
+    private Drop drop;
+    public Consumer(Drop drop) {
+        this.drop = drop;
+    }
+    public void run() {
+        Random random = new Random();
+        for (String message = drop.take();
+             ! message.equals("DONE");
+             message = drop.take()) {
+            System.out.format("MESSAGE RECEIVED: %s%n", message);
+            try {
+                Thread.sleep(random.nextInt(5000));
+            } catch (InterruptedException e) {}
+        }
+    }
+}
+public class ProducerConsumerExample {
+    public static void main(String[] args) {
+        Drop drop = new Drop();
+        (new Thread(new Producer(drop))).start();
+        (new Thread(new Consumer(drop))).start();
+    }
+}
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A concurrent application's ability to execute in a timely manner is known as its liveness. The most common kind of liveness problem is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deadlock,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and two other liveness problems, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>starvation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">livelock.
+Deadlock </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is saying 2 threads start an action accidentally at the same time which the action require couterpart to finish first.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Starvation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is saying 1 thread is taking too much resource time that it becomes the bottlebeck
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Livelock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is saying that 2 man meets in a narrow corridor...</t>
+    </r>
+  </si>
+  <si>
+    <t>Concurrency Usage</t>
+  </si>
+  <si>
+    <t>Webserver: Many thread read/write the web resource
+WhateverServer: same
+FileSystem</t>
+  </si>
+  <si>
+    <t>Concurrency: Employing Immutable Object to Lower the chance of thread corruption</t>
+  </si>
+  <si>
+    <t># An example without immutable object
+public class SynchronizedRGB {
+    // Values must be between 0 and 255.
+    private int red;
+    private int green;
+    private int blue;
+    private String name;
+    private void check(int red,
+                       int green,
+                       int blue) {
+        if (red &lt; 0 || red &gt; 255
+            || green &lt; 0 || green &gt; 255
+            || blue &lt; 0 || blue &gt; 255) {
+            throw new IllegalArgumentException();
+        }
+    }
+    public SynchronizedRGB(int red,
+                           int green,
+                           int blue,
+                           String name) {
+        check(red, green, blue);
+        this.red = red;
+        this.green = green;
+        this.blue = blue;
+        this.name = name;
+    }
+    public void set(int red,
+                    int green,
+                    int blue,
+                    String name) {
+        check(red, green, blue);
+        synchronized (this) {
+            this.red = red;
+            this.green = green;
+            this.blue = blue;
+            this.name = name;
+        }
+    }
+    public synchronized int getRGB() {
+        return ((red &lt;&lt; 16) | (green &lt;&lt; 8) | blue);
+    }
+    public synchronized String getName() {
+        return name;
+    }
+    public synchronized void invert() {
+        red = 255 - red;
+        green = 255 - green;
+        blue = 255 - blue;
+        name = "Inverse of " + name;
+    }
+}
+# An immutable version 
+final public class ImmutableRGB {
+    // Values must be between 0 and 255.
+    final private int red;
+    final private int green;
+    final private int blue;
+    final private String name;
+    private void check(int red,
+                       int green,
+                       int blue) {
+        if (red &lt; 0 || red &gt; 255
+            || green &lt; 0 || green &gt; 255
+            || blue &lt; 0 || blue &gt; 255) {
+            throw new IllegalArgumentException();
+        }
+    }
+    public ImmutableRGB(int red,
+                        int green,
+                        int blue,
+                        String name) {
+        check(red, green, blue);
+        this.red = red;
+        this.green = green;
+        this.blue = blue;
+        this.name = name;
+    }
+    public int getRGB() {
+        return ((red &lt;&lt; 16) | (green &lt;&lt; 8) | blue);
+    }
+    public String getName() {
+        return name;
+    }
+    public ImmutableRGB invert() {
+        return new ImmutableRGB(255 - red,
+                       255 - green,
+                       255 - blue,
+                       "Inverse of " + name);
+    }
+}
+# Advantage 
+For the first example, we must use sync statement between getters like:
+synchronized (color) {
+    int myColorInt = color.getRGB();
+    String myColorName = color.getName();
+} 
+But no need in the immutable version</t>
   </si>
 </sst>
 </file>
@@ -3753,13 +4076,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="33" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" style="2" customWidth="1"/>
@@ -3767,9 +4090,9 @@
     <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="33" customHeight="1">
+    <row r="1" spans="1:3" ht="32.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -3778,31 +4101,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="32.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+      <c r="C2" s="15" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="32.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="32.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
@@ -3811,42 +4134,42 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="32.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="4" customFormat="1" ht="32.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="4" customFormat="1" ht="32.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="4" customFormat="1" ht="33" customHeight="1">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="4" customFormat="1" ht="32.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -3855,31 +4178,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="33" customHeight="1">
+    <row r="9" spans="1:3" ht="32.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="33" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32.25" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="33" customHeight="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="32.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
@@ -3888,947 +4211,991 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="33" customHeight="1">
+    <row r="12" spans="1:3" ht="32.25" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="33" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="33" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="33" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="33" customHeight="1">
-      <c r="A16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="33" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="15" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="33" customHeight="1">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="33" customHeight="1">
-      <c r="A20" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="33" customHeight="1">
+    <row r="21" spans="1:3" ht="32.25" customHeight="1">
       <c r="A21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="33" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="33" customHeight="1">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="33" customHeight="1">
-      <c r="A24" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="33" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="15" t="s">
+    </row>
+    <row r="26" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="33" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="33" customHeight="1">
+    </row>
+    <row r="27" spans="1:3" ht="32.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C27" s="15" t="s">
+    </row>
+    <row r="28" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A28" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="33" customHeight="1">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="33" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="30" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A30" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A36" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A37" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A38" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A39" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A40" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A41" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A42" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A43" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A44" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A45" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A46" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A47" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A48" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A49" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A50" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A51" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A52" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A53" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A54" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A55" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A56" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="33" customHeight="1">
-      <c r="A30" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="33" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="33" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="33" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="33" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="33" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="33" customHeight="1">
-      <c r="A36" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="33" customHeight="1">
-      <c r="A37" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="33" customHeight="1">
-      <c r="A38" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="33" customHeight="1">
-      <c r="A39" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="33" customHeight="1">
-      <c r="A40" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="33" customHeight="1">
-      <c r="A41" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="33" customHeight="1">
-      <c r="A42" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="33" customHeight="1">
-      <c r="A43" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="33" customHeight="1">
-      <c r="A44" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="33" customHeight="1">
-      <c r="A45" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="33" customHeight="1">
-      <c r="A46" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="33" customHeight="1">
-      <c r="A47" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="33" customHeight="1">
-      <c r="A48" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="33" customHeight="1">
-      <c r="A49" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="33" customHeight="1">
-      <c r="A50" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="33" customHeight="1">
-      <c r="A51" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C51" s="15" t="s">
+      <c r="C56" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A57" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="33" customHeight="1">
-      <c r="A52" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="33" customHeight="1">
-      <c r="A53" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="33" customHeight="1">
-      <c r="A54" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="33" customHeight="1">
-      <c r="A55" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B55" s="2" t="s">
+      <c r="B57" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A58" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A59" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A60" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A61" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A62" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A63" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="C55" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="71.45" customHeight="1">
-      <c r="A56" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="33" customHeight="1">
-      <c r="A57" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="A58" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="33" customHeight="1">
-      <c r="A59" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="33" customHeight="1">
-      <c r="A60" s="15" t="s">
-        <v>200</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="C60" s="15" t="s">
+      <c r="B63" s="15" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="33" customHeight="1">
-      <c r="A61" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="33" customHeight="1">
-      <c r="A62" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="C62" s="16" t="s">
+      <c r="C63" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A64" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A65" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="33" customHeight="1">
-      <c r="A63" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B63" s="15" t="s">
+      <c r="C65" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A66" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="C63" s="15" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="33" customHeight="1">
-      <c r="A64" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B64" s="15" t="s">
+      <c r="B66" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A67" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B67" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C67" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A68" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A69" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A70" s="15" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="33" customHeight="1">
-      <c r="A65" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="33" customHeight="1">
-      <c r="A66" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>216</v>
-      </c>
-      <c r="C66" s="15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="33" customHeight="1">
-      <c r="A67" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="33" customHeight="1">
-      <c r="A68" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="33" customHeight="1">
-      <c r="A69" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="33" customHeight="1">
-      <c r="A70" s="15" t="s">
+      <c r="B70" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A71" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="B70" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="C70" s="15" t="s">
+      <c r="B71" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C71" s="15" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="33" customHeight="1">
-      <c r="A71" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="C71" s="15" t="s">
+    <row r="72" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A72" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" s="15" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="33" customHeight="1">
-      <c r="A72" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B72" s="15" t="s">
+      <c r="C72" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="C72" s="15" t="s">
+    </row>
+    <row r="73" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A73" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="B73" s="15" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="33" customHeight="1">
-      <c r="A73" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B73" s="15" t="s">
+      <c r="C73" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="C73" s="15" t="s">
+    </row>
+    <row r="74" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A74" s="15" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" ht="33" customHeight="1">
-      <c r="A74" s="15" t="s">
+      <c r="B74" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="B74" s="15" t="s">
+      <c r="C74" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="C74" s="15" t="s">
+    </row>
+    <row r="75" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A75" s="15" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="33" customHeight="1">
-      <c r="A75" s="15" t="s">
+      <c r="B75" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C75" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="B75" s="15" t="s">
+    </row>
+    <row r="76" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A76" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A77" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B77" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C75" s="15" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="33" customHeight="1">
-      <c r="A76" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="C76" s="15" t="s">
+      <c r="C77" s="15" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="33" customHeight="1">
-      <c r="A77" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="C77" s="15" t="s">
+    <row r="78" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A78" s="15" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="33" customHeight="1">
-      <c r="A78" s="15" t="s">
+      <c r="B78" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="B78" s="15" t="s">
+      <c r="C78" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="C78" s="15" t="s">
+    </row>
+    <row r="79" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A79" s="15" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="33" customHeight="1">
-      <c r="A79" s="15" t="s">
+      <c r="B79" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="B79" s="15" t="s">
+      <c r="C79" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A80" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="C79" s="15" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="33" customHeight="1">
-      <c r="A80" s="15" t="s">
+      <c r="B80" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="C80" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="C80" s="15" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="180.75">
+    </row>
+    <row r="81" spans="1:3" ht="32.25" customHeight="1">
       <c r="A81" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B81" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="B81" s="15" t="s">
+      <c r="C81" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A82" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B82" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="C82" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A83" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A84" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A85" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C85" s="15" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="57">
-      <c r="A82" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="57">
-      <c r="A83" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="147">
-      <c r="A84" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B84" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="C84" s="15" t="s">
+    <row r="86" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A86" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C86" s="15" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="90.75">
-      <c r="A85" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B85" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="113.25">
-      <c r="A86" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B86" s="15" t="s">
+    <row r="87" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A87" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B87" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C87" s="15" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="174" customHeight="1">
-      <c r="A87" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B87" s="15" t="s">
+    <row r="88" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A88" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B88" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="C87" s="15" t="s">
+      <c r="C88" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A89" s="15" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" ht="158.25">
-      <c r="A88" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B88" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="C88" s="15" t="s">
+      <c r="B89" s="15" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" ht="33" customHeight="1">
-      <c r="A89" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B89" s="15" t="s">
+      <c r="C89" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="C89" s="15" t="s">
+    </row>
+    <row r="90" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A90" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B90" s="15" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="33" customHeight="1">
-      <c r="A90" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B90" s="15" t="s">
+      <c r="C90" s="15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A91" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B91" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="C90" s="15" t="s">
+      <c r="C91" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A92" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B92" s="15" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" ht="33" customHeight="1">
-      <c r="A91" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="33" customHeight="1">
-      <c r="A92" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B92" s="15" t="s">
+      <c r="C92" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="C92" s="15" t="s">
+    </row>
+    <row r="93" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A93" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C93" s="15" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="64.5" customHeight="1">
-      <c r="A93" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B93" s="15" t="s">
+    <row r="94" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A94" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A95" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B95" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="C95" s="15" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="33" customHeight="1">
-      <c r="A94" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B94" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="C94" s="15" t="s">
+    <row r="96" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A96" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C96" s="15" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="33" customHeight="1">
-      <c r="A95" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B95" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="33" customHeight="1">
-      <c r="A96" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B96" s="15" t="s">
+    <row r="97" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A97" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B97" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="C96" s="15" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="33" customHeight="1">
-      <c r="A97" s="15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B97" s="15" t="s">
+      <c r="C97" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="C97" s="15" t="s">
-        <v>289</v>
+    </row>
+    <row r="98" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A98" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="C98" s="15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A99" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B99" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="C99" s="17" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A100" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A101" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="C101" s="15" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4856,190 +5223,190 @@
   <sheetData>
     <row r="1" spans="1:1" ht="37.5">
       <c r="A1" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="93.75">
       <c r="A5" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75">
       <c r="A7" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75">
       <c r="A8" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75">
       <c r="A9" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75">
       <c r="A10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75">
       <c r="A11" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="60">
       <c r="A13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="39">
       <c r="A15" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="C20" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75">
       <c r="A21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>81</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30">
       <c r="A23" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>85</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="C24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>88</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="46.5">
       <c r="A25" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C25" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>91</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30">
       <c r="A26" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -5069,12 +5436,12 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60">
@@ -5082,10 +5449,10 @@
         <v>42816</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5093,7 +5460,7 @@
         <v>42814</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45">
@@ -5101,10 +5468,10 @@
         <v>42772</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -5112,10 +5479,10 @@
         <v>42772</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45">
@@ -5123,7 +5490,7 @@
         <v>42754</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>

</xml_diff>

<commit_message>
Add java entry on standard comment style for classed and methods
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="302">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -3552,6 +3552,56 @@
     String myColorName = color.getName();
 } 
 But no need in the immutable version</t>
+  </si>
+  <si>
+    <t>comment style (class)</t>
+  </si>
+  <si>
+    <t>comment style (method)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    /**
+     * Skips over and discards &lt;code&gt;n&lt;/code&gt; bytes of data from the
+     * input stream.
+     *
+     * &lt;p&gt;The &lt;code&gt;skip&lt;/code&gt; method may, for a variety of
+     * reasons, end up skipping over some smaller number of bytes,
+     * possibly &lt;code&gt;0&lt;/code&gt;. If &lt;code&gt;n&lt;/code&gt; is negative, an
+     * &lt;code&gt;IOException&lt;/code&gt; is thrown, even though the &lt;code&gt;skip&lt;/code&gt;
+     * method of the {@link InputStream} superclass does nothing in this case.
+     * The actual number of bytes skipped is returned.
+     *
+     * &lt;p&gt;This method may skip more bytes than are remaining in the backing
+     * file. This produces no exception and the number of bytes skipped
+     * may include some number of bytes that were beyond the EOF of the
+     * backing file. Attempting to read from the stream after skipping past
+     * the end will result in -1 indicating the end of the file.
+     *
+     * @param      n   the number of bytes to be skipped.
+     * @return     the actual number of bytes skipped.
+     * @exception  IOException  if n is negative, if the stream does not
+     *             support seek, or if an I/O error occurs.
+     */
+    public native long skip(long n) throws IOException...</t>
+  </si>
+  <si>
+    <t>/**
+ * A &lt;code&gt;FileInputStream&lt;/code&gt; obtains input bytes
+ * from a file in a file system. What files
+ * are  available depends on the host environment.
+ *
+ * &lt;p&gt;&lt;code&gt;FileInputStream&lt;/code&gt; is meant for reading streams of raw bytes
+ * such as image data. For reading streams of characters, consider using
+ * &lt;code&gt;FileReader&lt;/code&gt;.
+ *
+ * @author  Arthur van Hoff
+ * @see     java.io.File
+ * @see     java.io.FileDescriptor
+ * @see     java.io.FileOutputStream
+ * @see     java.nio.file.Files#newInputStream
+ * @since   JDK1.0
+ */
+public class FileInputStream extends InputStream ...</t>
   </si>
 </sst>
 </file>
@@ -4076,10 +4126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+      <selection activeCell="B106" sqref="B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
@@ -5196,6 +5246,28 @@
       </c>
       <c r="C101" s="15" t="s">
         <v>297</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A102" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A103" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entries on RTFL:Concurrency High Level
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="316">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -3602,6 +3602,93 @@
  * @since   JDK1.0
  */
 public class FileInputStream extends InputStream ...</t>
+  </si>
+  <si>
+    <t>More on InputStream vs Reader</t>
+  </si>
+  <si>
+    <t>Reading the Core Java Book, found out that the InputStream is introduced at 1.0, and Reader are introduced later. Basicly InputStream tackle data at a byte level, while Reader tackle data at double-byte/ aka Unicode level. 
+The author suggested that we should try to use Reader/Writer at most case, but use the inputStream/ OutputStream when the former is not applicable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concurrency: High Level </t>
+  </si>
+  <si>
+    <t>Thread and Runnable are in java.lang package. But iits lowlevel, to have higher level abstraction, new classes are introduced in _java.util.concurrent package_ after JDK5. 
+At the same time, new concurrent package also add new members to the Java Collections Framework.</t>
+  </si>
+  <si>
+    <t>Concurrency: High Level- Core Interface</t>
+  </si>
+  <si>
+    <t># Core Interface Introduction
+## Executor interface
+Provide the core interface with only one method: execute. (e.g. e.execute(r:Runnable);)
+## ExecutorService interface
+Extends the Executor interface, provide more action on lifecycle management of the service itself and its thread pool memebrs.
+## ScheduledExecutorService interface
+Extends the ExecutorService and provide scheduling ability
+# 2 main ideas in new concurrent pacakge
+1. Runnable類從主體變成客體. 以往是new Thread(r).start(); 現在是: executor.execute(r); 好處是應用這個build設計模式使executor的新功能可重用, 強大!
+2. ThreadPool concept is introduced to ExecutorService. Basically, a lot of impl of ExecutorService is thread pools. 這是使用Builder pattern 後才使其成為可能.</t>
+  </si>
+  <si>
+    <t>Concurency: High Level- Executors Factory</t>
+  </si>
+  <si>
+    <t>Executors(java.util.concurrency.Executors) is a factory that provides different ExecutorService. They are:
+* CachedThreadPool
+* FixedThreadPool
+* ScheduledThreadPool
+* SingleThreadExecutor</t>
+  </si>
+  <si>
+    <t>Concurrency: High Level- Fork/Join Framework</t>
+  </si>
+  <si>
+    <t>Concurrency: High Level- new members of Java Collection Framework</t>
+  </si>
+  <si>
+    <t>Concurrency: High Level- Atomic package</t>
+  </si>
+  <si>
+    <t>Fork/Join Framework is introduced to allow the work-stealing algroithm: one free-of-work thread can steal works from another busy thread. 
+To enable this framework, refactor the code to follow below pseudo code:
+```
+if (my portion of the work is small enough)
+  do the work directly
+else
+  split my work into two pieces
+  invoke the two pieces and wait for the results
+```
+For detail usage, reference the manual</t>
+  </si>
+  <si>
+    <t>New members are:
+* BlockingQueue: defines a first-in-first-out data structure that blocks or times out when you attempt to add to a full queue, or retrieve from an empty queue.
+* ConcurrentMap: a subinterface of java.util.Map that defines useful atomic operations. These operations remove or replace a key-value pair only if the key is present, or add a key-value pair only if the key is absent. Making these operations atomic helps avoid synchronization. The standard general-purpose implementation of ConcurrentMap is ConcurrentHashMap, which is a concurrent analog of HashMap.
+* ConcurrentNavigableMap: a subinterface of ConcurrentMap that supports approximate matches. The standard general-purpose implementation of ConcurrentNavigableMap is ConcurrentSkipListMap, which is a concurrent analog of TreeMap.</t>
+  </si>
+  <si>
+    <t>Atomic package (java.util.concurrency.atomic) provides handy utils for atomic operation. In previous session, the integer counter method increment() adds the **synchronize** keyword to atomicize itself. 
+```
+class SynchronizedCounter {
+    private int c = 0;
+    public synchronized void increment() {   c++;   }
+    public synchronized void decrement() {   c--;    }
+    public synchronized int value() {    return c;    }
+}
+```
+With atomic package, this turns into:
+```
+import java.util.concurrent.atomic.AtomicInteger;
+class AtomicCounter {
+    private AtomicInteger c = new AtomicInteger(0);
+    public void increment() {        c.incrementAndGet();    }
+    public void decrement() {        c.decrementAndGet();    }
+    public int value() {        return c.get();    }
+}
+```</t>
   </si>
 </sst>
 </file>
@@ -4126,10 +4213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
@@ -5268,6 +5355,83 @@
       </c>
       <c r="C103" s="15" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A104" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A105" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B105" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="C105" s="15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A106" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B106" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="C106" s="15" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A107" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B107" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="C107" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A108" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B108" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="C108" s="15" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A109" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B109" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A110" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B110" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry on RTFM: Platform Environment
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="322">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -3690,12 +3690,112 @@
 }
 ```</t>
   </si>
+  <si>
+    <t>Platform Environment: Configuration Utilities</t>
+  </si>
+  <si>
+    <t>JDK provides utils for configuration setting:
+1. Properties
+2. JVM injected command-line arguments (get from args)
+3. Get OS environment vars by : Map&lt;String, String&gt; env = System.getenv();
+4. Others utils like Preferences API, mainifest in a jar directory, etc.</t>
+  </si>
+  <si>
+    <t>Platform Environment: System Utilities</t>
+  </si>
+  <si>
+    <t>Some of utils provided by final static class **System** were covered in previous section, but there are some not covered and here they are:
+1. System.in: used for user to read input from command line as user interface
+2. System.getProperty(String): return the property value
+3. System.getSecurityManager(): security manager is default null in standalone application but available in frameworks like the java Applet. For example, in standalone app, statement `reader = new FileReader("xanadu.txt");` might work well but in Applet, a SecurityException wil be thrown (this is true even when invoking a method that isn't documented as throwing SecurityException)
+4. Other System utils like System.currentTimeMillis(), System.arrayCopy(), etc</t>
+  </si>
+  <si>
+    <t>Platform Environment: PATH&amp; CLASSPATH</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"># Path
+Not necessarily needed, mainly for persist convenience. 
+# Classpath
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CLASSPATH</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> variable is one way to tell applications, including the JDK tools, where to look for user classes. (Classes that are part of the JRE, JDK platform, and extensions should be defined through other means, such as the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bootstrap class path</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or the extensions directory.)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* -cp can be used to override default classpath
+* default classpath of jvm is "."
+* Class path wildcards allow you to include an entire directory of .jar files in the class path without explicitly naming them individually
+For more on classpath, read the _Setting the Class Path_ technical note.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3800,6 +3900,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -4213,9 +4321,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
@@ -5432,6 +5540,39 @@
       </c>
       <c r="C110" s="15" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A111" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B111" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A112" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B112" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A113" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry on regex trail
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="327">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -3789,6 +3789,44 @@
 * Class path wildcards allow you to include an entire directory of .jar files in the class path without explicitly naming them individually
 For more on classpath, read the _Setting the Class Path_ technical note.</t>
     </r>
+  </si>
+  <si>
+    <t>The syntax impl is most similar to perl among all differnet regex util like grep, awk and etc. Three major class is used in java.util.regex package:
+1. Pattern: represent the compiled pattern, construct by static factory method Pattern.compile(String regex)
+2. Matcher: represent the one who has the knowlege to match string with pattern. its construct by objPattern.matcher(String str_to_search)
+3. PatternSyntaxException</t>
+  </si>
+  <si>
+    <t>Regex: Syntax in java</t>
+  </si>
+  <si>
+    <t>Regex: Example</t>
+  </si>
+  <si>
+    <t>Pattern pattern = Pattern.compile("my.*[a-z]+");
+Matcher matcher = pattern.matcher("A string to be searched");
+boolean found = false;
+ while (matcher.find()) {
+                console.format("I found the text" +
+                    " \"%s\" starting at " +
+                    "index %d and ending at index %d.%n",
+                    matcher.group(),
+                    matcher.start(),
+                    matcher.end());
+                found = true;
+ }</t>
+  </si>
+  <si>
+    <t>Below topics are covered in the manual:
+1.  regex of Character ([a-z])
+2.  regex of Predefined Character (\d, \D)
+3. regex of qualifier (X?, X*, X+)
+4. Capturing Group ((A)*(B)(C)+)
+5. regex of boundary (^, $)
+6. manual of Pattern
+7. manual of Matcher
+8. manual of XXXException
+9. how to match unicode (\uxxxx)</t>
   </si>
 </sst>
 </file>
@@ -4321,10 +4359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A107" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
@@ -5573,6 +5611,39 @@
       </c>
       <c r="C113" s="15" t="s">
         <v>321</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A114" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A115" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B115" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A116" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B116" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="C116" s="15" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry on Aggregate Operation(JDK8)
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="333">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -3827,6 +3827,58 @@
 7. manual of Matcher
 8. manual of XXXException
 9. how to match unicode (\uxxxx)</t>
+  </si>
+  <si>
+    <t>Collection: Interface</t>
+  </si>
+  <si>
+    <t># Core collection interfaces
+Collection
+Collection -&gt; Set
+Collection -&gt; Set -&gt; SortedSet
+Collection -&gt; List
+Collection -&gt; Queue
+Collection -&gt; Deque
+Map
+Map -&gt; SortedMap
+(note: Map is not a collection technically)</t>
+  </si>
+  <si>
+    <t>Collection: Interface (2)</t>
+  </si>
+  <si>
+    <t># Some bullet points:
+* Deque is like a queue but allow both end insert/remove
+* TreeSet is a set that sorted by natural order (or comparator), and it guarrantee log2(n) speed
+* Aggregate function is capable of performing filtering for collections. Introduced after JDK 8
+* Aggregate function stream() and ParralelStream() are same function for single and multiple cores.
+* Class Collections is a util class.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggregate Operations </t>
+  </si>
+  <si>
+    <t># Introduction
+Aggregate Operation alike the hadoop **map/reduce**. It is friendly to distributed programming, and so does the aggregate operation in java. Observe:
+c.stream()
+  .filter(xxx)    // **mapper**: select the result (and sort?)
+  .forEach(xxx)  // **reducer**: process the data
+# Example
+roster
+    .stream()
+    .forEach(e -&gt; System.out.println(e.getName());
+roster
+    .stream()
+    .filter(e -&gt; e.getGender() == Person.Sex.MALE)   //filter return another stream
+    .forEach(e -&gt; System.out.println(e.getName()));
+double average = roster
+    .stream()
+    .filter(p -&gt; p.getGender() == Person.Sex.MALE)
+    .mapToInt(Person::getAge)
+    .average()
+    .getAsDouble();
+# Differences between iterator
+Though with similar functionality, aggregate operations is based on Stream (java.util.stream.Stream [jdk8]), and since aggregate operations use *internal delegation* to tell what kind of collection it is and how to iterate, so that it allows *parallel operations*.</t>
   </si>
 </sst>
 </file>
@@ -4359,10 +4411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C116"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
@@ -5644,6 +5696,44 @@
       </c>
       <c r="C116" s="15" t="s">
         <v>325</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A117" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A118" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A119" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="C119" s="15" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A120" s="15" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry about RTFM: Collection, finish collection
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="343">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -3855,9 +3855,6 @@
 * Class Collections is a util class.</t>
   </si>
   <si>
-    <t xml:space="preserve">Aggregate Operations </t>
-  </si>
-  <si>
     <t># Introduction
 Aggregate Operation alike the hadoop **map/reduce**. It is friendly to distributed programming, and so does the aggregate operation in java. Observe:
 c.stream()
@@ -3879,6 +3876,94 @@
     .getAsDouble();
 # Differences between iterator
 Though with similar functionality, aggregate operations is based on Stream (java.util.stream.Stream [jdk8]), and since aggregate operations use *internal delegation* to tell what kind of collection it is and how to iterate, so that it allows *parallel operations*.</t>
+  </si>
+  <si>
+    <t>Lambda Expression</t>
+  </si>
+  <si>
+    <t># What is it 
+Lambda expression looks like a method declaration, you can consider lambda expressions as anonymous methods- methods without a name.
+# Where can use
+## To replace any anonymous inner class that has only **single method interface**. In below example, tester1 and tester2 are equivalent.
+```
+interface Foo{
+    boolean check(T t);
+}
+public void main(){
+    tester1.setFoo(new Foo{
+        @Override
+        public boolean check(T t){
+            return t.foobar();
+        }
+    });
+    tester2.setFoo( t -&gt; t.foobar() );
+}
+```
+## To pass into **Aggregate Operations** that accept Lambda Expressions as parameters
+```
+roster
+    .stream()
+    .filter(p -&gt; p.getGender() == Person.Sex.MALE &amp;&amp; p.getAge() &gt;= 18 &amp;&amp; p.getAge() &lt;= 25)
+    .map(p -&gt; p.getEmailAddress())
+    .forEach(email -&gt; System.out.println(email));
+```
+# Syntax
+For below code, the statement after -&gt; will treat as a return statement automatically:
+` p -&gt; p.getAge() `
+For below code, return is implicitly decare:
+```
+p -&gt; { 
+    p.refresh();
+    p.increment();
+    return p.getAge();
+}
+```</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collection: Aggregate Operations </t>
+  </si>
+  <si>
+    <t>Collection: Impls</t>
+  </si>
+  <si>
+    <t># Implementations of Collection Interface
+* Impl only affect performance, not feature
+* Vector and Hashtable are legacy collections, they are synchonized. But lastest alternatives ArrayList and HashMap are not, so to reduce sync overhead and unnecessary feature. " In general, it is good API design practice not to make users pay for a feature they don't use."
+* If thread-safe collections needed:
+    * Collection impl from java.util.concurrent (offers much higher concurrency than sync wrapping collection)
+    * Synchronization wrapper to wrap your collections
+# Commonly use general purpose collection implementations
+* For the Set interface, HashSet is the most commonly used implementation.
+* For the List interface, ArrayList is the most commonly used implementation.
+* For the Map interface, HashMap is the most commonly used implementation.
+* For the Queue interface, LinkedList is the most commonly used implementation.
+* For the Deque interface, ArrayDeque is the most commonly used implementation.</t>
+  </si>
+  <si>
+    <t>Collection: Algorithms</t>
+  </si>
+  <si>
+    <t>The collection interface does not carry operation itself (sort, search, shuffle and etc). These operation and algorithms are provided in Collections:
+Collections.min(List, Comparator)
+Collections.max(List, Comparator)
+Collections.sort(List, Comparator)
+Collections.binarySearch(List, T)</t>
+  </si>
+  <si>
+    <t>Collection: Custom Collection Design</t>
+  </si>
+  <si>
+    <t>AbstractList is provided to resue for new Impl of Collections. As long as user impl the constructor, the get, the set and the size methods, the other bulk operations are provided in AbstractList already.
+For other interface, the same principle applies.</t>
+  </si>
+  <si>
+    <t>Collection: Inter-operability</t>
+  </si>
+  <si>
+    <t># Compatibility 
+* Upward Compatibility: Get array from oldMethod() and pass to newMethod with Arrays.asList() that construct an List based on the array
+* Backward Compatibility: Get collection from newMethod() and "down-grade" it to array with List.toArray() method and pass the arry to oldMethod()
+* I learnt that 兼容性在不同語境下有不同含義. 在JVM層面下, 那就是JRE7可否運行JDK6的程序這樣的問題. 而在代碼層面, 則是接口過渡問題. 如上所述, 只要能夠將舊接口的訊息不失真地轉移到新接口, 則稱其Upward Compability; 而新接口的東西, 反之能轉換回舊接口可識別的訊息, 則稱Backward Compatibility</t>
   </si>
 </sst>
 </file>
@@ -4411,10 +4496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
@@ -5725,15 +5810,65 @@
         <v>261</v>
       </c>
       <c r="B119" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="C119" s="15" t="s">
         <v>331</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="32.25" customHeight="1">
       <c r="A120" s="15" t="s">
         <v>261</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="C120" s="15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A121" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B121" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C121" s="15" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A122" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="C122" s="15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A123" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C123" s="15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A124" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="C124" s="15" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add java entry about i18n(internationalization)
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="349">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -3964,6 +3964,75 @@
 * Upward Compatibility: Get array from oldMethod() and pass to newMethod with Arrays.asList() that construct an List based on the array
 * Backward Compatibility: Get collection from newMethod() and "down-grade" it to array with List.toArray() method and pass the arry to oldMethod()
 * I learnt that 兼容性在不同語境下有不同含義. 在JVM層面下, 那就是JRE7可否運行JDK6的程序這樣的問題. 而在代碼層面, 則是接口過渡問題. 如上所述, 只要能夠將舊接口的訊息不失真地轉移到新接口, 則稱其Upward Compability; 而新接口的東西, 反之能轉換回舊接口可識別的訊息, 則稱Backward Compatibility</t>
+  </si>
+  <si>
+    <t>JAR</t>
+  </si>
+  <si>
+    <t># JAR command
+Usage: jar {ctxui}[vfmn0PMe] [jar-file] [manifest-file] [entry-point] [-C dir] files ...
+Options:
+    -c  create new archive
+    -t  list table of contents for archive
+    -x  extract named (or all) files from archive
+    -u  update existing archive
+    -v  generate verbose output on standard output
+    -f  specify archive file name
+    -m  include manifest information from specified manifest file
+    -n  perform Pack200 normalization after creating a new archive
+    -e  specify application entry point for stand-alone application
+        bundled into an executable jar file
+    -0  store only; use no ZIP compression
+    -P  preserve leading '/' (absolute path) and ".." (parent directory) components from file names
+    -M  do not create a manifest file for the entries
+    -i  generate index information for the specified jar files
+    -C  change to the specified directory and include the following file
+If any file is a directory then it is processed recursively.
+The manifest file name, the archive file name and the entry point name are
+specified in the same order as the 'm', 'f' and 'e' flags.
+Example 1: to archive two class files into an archive called classes.jar:
+       jar cvf classes.jar Foo.class Bar.class
+Example 2: use an existing manifest file 'mymanifest' and archive all the
+           files in the foo/ directory into 'classes.jar':
+       jar cvfm classes.jar mymanifest -C foo/ .</t>
+  </si>
+  <si>
+    <t>JAR: more on jar</t>
+  </si>
+  <si>
+    <t>We can use "jar" command to add info to manifest file from another file or from command line args. But with a build tool like ant or maven, this is replace by cnetralized project doc like "pom.xml"</t>
+  </si>
+  <si>
+    <t>i18n</t>
+  </si>
+  <si>
+    <t>i18n is the abbreviation of internationalization. Similiarly, l10n is the abbreviation of localization. Util ResourceBundle and Locale are provided in JDK to read properties from bundle file in a certainly formating like "MessagesBundle_fr_FR.properties" and "MessagesBundle_en_US.properties" with code below:
+```
+import java.util.*;
+public class I18NSample {
+    static public void main(String[] args) {
+        String language;
+        String country;
+        if (args.length != 2) {
+              return; //invalid number of ags
+        } else {
+            language = new String(args[0]);
+            country = new String(args[1]);
+        }
+        Locale currentLocale = new Locale(language, country);
+        ResourceBundle messages = ResourceBundle.getBundle("MessagesBundle", currentLocale);
+        System.out.println(messages.getString("greetings"));
+        System.out.println(messages.getString("inquiry"));
+        System.out.println(messages.getString("farewell"));
+    }
+}
+```
+While properties file follow classic format:
+```
+greetings = Bonjour.
+farewell = Au revoir.
+inquiry = Comment allez-vous?
+```</t>
   </si>
 </sst>
 </file>
@@ -4496,10 +4565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
@@ -5869,6 +5938,39 @@
       </c>
       <c r="C124" s="15" t="s">
         <v>342</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A125" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="C125" s="15" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A126" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="C126" s="15" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A127" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="C127" s="15" t="s">
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add security/ javabean/ extension/ generic, and Refactoring exp
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="360">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -4033,6 +4033,240 @@
 farewell = Au revoir.
 inquiry = Comment allez-vous?
 ```</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Jave Bean</t>
+  </si>
+  <si>
+    <t>Static Method? Throughts on refactoring</t>
+  </si>
+  <si>
+    <t>Show what is java bean(POLO).</t>
+  </si>
+  <si>
+    <t>Introduce the common methodology in security:
+1. Security setting for JVM:
+When use java (the jvm command) to run java application, by dedault, invoke no security restriction. But with `java -Djava.security.manager {app_name}` inovke the security manager. There are policy file that can be injected to this security manager. Read more from the trail.
+2. Exchanging Code or Document, the common methodology
+When exchange code/file between entities, one should prove his/her identity. 表明自己身份可以通過Sign來完成:
+    * Use private key to sign the file
+    * Supply the receipent the signed file and your certificate (contains your public key)
+    * 因為RSA非對稱加密原理, 收件人可以用Public key解密到你用Private Key加密的文件, 從而證明你是真正的Public key + Priavte key Owner. 
+接下來問題便是如何證明此公匙未被偷換, Public key 被包含在Certificate中, Certificate 包:
+    * Owner Name (你)
+    * Owner Public key
+    * A signed data by Certificate Authority(CA)
+    * CA Name
+此CA Vouch for your public key's integrity. But Next question moves to the integrity of this CA. So we keep on verifying public key's integrity using its voucher CA's public key... we continue this "TRUST CHAIN" until we verify the end of the chain with a proven public key. 一旦證實, 則鏈中所有Public key都可以被Mark作Proven. 這些統統都存到本地的Keystore中.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">When I am refactoring the qrc-decoder, I separate the actions toward cheque from the Jframe. And I realize that those operations are actually not supposed to be in the Cheque class. So I start to think whether I should put it insider the Cheque class as static method, or should I create a new class Cheques that owns several static method?
+Here is the logical steps I took:
+1. Refine your abstraction floorplan
+2. According to the floorplan, arrange the properties to different class first
+3. For actions/operations, arrang them to class if:
+    * </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> param needed can be found in class A property set, and the action itself logically makes sense to be in class A accroding to floorplan -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>non-static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> method in class A
+    * </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOT ALL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> param needed can be found in class A property set, and the action itself logically makes sense to be in class A accroding to floorplan -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">static </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">method in class A
+    * The action itself logically makes </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sense to be in class A accroding to floorplan -&gt; static method(A injected and others) in class NEW</t>
+    </r>
+  </si>
+  <si>
+    <t>If any jar packages are put into $JAVA_HOME/jre/lib/ext, this jar will be treated as the extension of JRE which enjoys:
+* loaded without need to any implicit declaration in jvm -cp
+* no need to add as dependency in development
+(p.s. After JDK6, a public path is also included as acceptable java extension folder:
+Solaris: /usr/jdk/packages/lib/ext
+Linux: /usr/java/packages/lib/ext
+Windows: %SystemRoot%\Sun\Java\lib\ext)</t>
+  </si>
+  <si>
+    <t>Extension Mechanism (1)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The packages loading sequence of JVM:
+0. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Bootstrap classes: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">the runtime classes in rt.jar, internationalization classes in i18n.jar, and others.
+1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Installed extensions: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">classes in JAR files in the lib/ext directory of the JRE, and in the system-wide, platform-specific extension directory.
+2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The class path: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>classes, including classes in JAR files, on paths specified by the system property java.class.path. If a JAR file on the class path has a manifest with the Class-Path attribute, JAR files specified by the Class-Path attribute will be searched also. By default, the java.class.path property's value is ., the current directory. You can change the value by using the -classpath or -cp command-line options, or setting the CLASSPATH environment variable. The command-line options override the setting of the CLASSPATH environment variable.</t>
+    </r>
+  </si>
+  <si>
+    <t>Skipped.</t>
+  </si>
+  <si>
+    <t>Generic</t>
   </si>
 </sst>
 </file>
@@ -4216,7 +4450,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4263,6 +4497,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4565,10 +4802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
@@ -5971,6 +6208,72 @@
       </c>
       <c r="C127" s="15" t="s">
         <v>348</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A128" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B128" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="C128" s="18" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A129" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B129" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="C129" s="15" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A130" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B130" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="C130" s="18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A131" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B131" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="C131" s="15" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A132" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B132" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="C132" s="15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A133" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="B133" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="C133" s="15" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add JVM options details to java lib
</commit_message>
<xml_diff>
--- a/java_lib.xlsx
+++ b/java_lib.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="9720" windowHeight="12540"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="369">
   <si>
     <t>GSON</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -4267,6 +4267,190 @@
   </si>
   <si>
     <t>Generic</t>
+  </si>
+  <si>
+    <t>JVM</t>
+  </si>
+  <si>
+    <t>JVM Options Overview</t>
+  </si>
+  <si>
+    <t>JVM Standard Options</t>
+  </si>
+  <si>
+    <t>JVM Non-standard Options (Xoption)</t>
+  </si>
+  <si>
+    <t>JVM Advanced Options (XXoption)</t>
+  </si>
+  <si>
+    <t># XXOption Category
+* __Behavioral options__ change the basic behavior of the VM.
+* Garbage First (G1) Garbage Collection Options
+* __Performance tuning options__ are knobs which can be used to tune VM performance.
+* __Debugging options__ generally enable tracing, printing, or output of VM information.
+# Behavioral Options:
+-XX:-AllowUserSignalHandlers Do not complain if the application installs signal handlers. (Relevant to Solaris and Linux only.)
+-XX:AltStackSize=16384 Alternate signal stack size (in Kbytes). (Relevant to Solaris only, removed from 5.0.)
+-XX:-DisableExplicitGC By default calls to System.gc() are enabled (-XX:-DisableExplicitGC). Use -XX:+DisableExplicitGC to disable calls to System.gc(). Note that the JVM still performs garbage collection when necessary.
+-XX:+FailOverToOldVerifier Fail over to old verifier when the new type checker fails. (Introduced in 6.)
+-XX:+HandlePromotionFailure The youngest generation collection does not require a guarantee of full promotion of all live objects. (Introduced in 1.4.2 update 11) [5.0 and earlier: false.]
+-XX:+MaxFDLimit Bump the number of file descriptors to max. (Relevant  to Solaris only.)
+-XX:PreBlockSpin=10 Spin count variable for use with -XX:+UseSpinning. Controls the maximum spin iterations allowed before entering operating system thread synchronization code. (Introduced in 1.4.2.)
+-XX:-RelaxAccessControlCheck Relax the access control checks in the verifier. (Introduced in 6.)
+-XX:+ScavengeBeforeFullGC Do young generation GC prior to a full GC. (Introduced in 1.4.1.)
+-XX:+UseAltSigs Use alternate signals instead of SIGUSR1 and SIGUSR2 for VM internal signals. (Introduced in 1.3.1 update 9, 1.4.1. Relevant to Solaris only.)
+-XX:+UseBoundThreads Bind user level threads to kernel threads. (Relevant to Solaris only.)
+-XX:-UseConcMarkSweepGC Use concurrent mark-sweep collection for the old generation. (Introduced in 1.4.1)
+-XX:+UseGCOverheadLimit Use a policy that limits the proportion of the VM's time that is spent in GC before an OutOfMemory error is thrown. (Introduced in 6.)
+-XX:+UseLWPSynchronization Use LWP-based instead of thread based synchronization. (Introduced in 1.4.0. Relevant to Solaris only.)
+-XX:-UseParallelGC Use parallel garbage collection for scavenges. (Introduced in 1.4.1)
+-XX:-UseParallelOldGC Use parallel garbage collection for the full collections. Enabling this option automatically sets -XX:+UseParallelGC. (Introduced in 5.0 update 6.)
+-XX:-UseSerialGC Use serial garbage collection. (Introduced in 5.0.)
+-XX:-UseSpinning Enable naive spinning on Java monitor before entering operating system thread synchronizaton code. (Relevant to 1.4.2 and 5.0 only.) [1.4.2, multi-processor Windows platforms: true]
+-XX:+UseTLAB Use thread-local object allocation (Introduced in 1.4.0, known as UseTLE prior to that.) [1.4.2 and earlier, x86 or with -client: false]
+-XX:+UseSplitVerifier Use the new type checker with StackMapTable attributes. (Introduced in 5.0.)[5.0: false]
+-XX:+UseThreadPriorities Use native thread priorities.
+-XX:+UseVMInterruptibleIO Thread interrupt before or with EINTR for I/O operations results in OS_INTRPT. (Introduced in 6. Relevant to Solaris only.)
+# Garbage Collection Options
+-XX:+UseG1GC Use the Garbage First (G1) Collector
+-XX:MaxGCPauseMillis=n Sets a target for the maximum GC pause time. This is a soft goal, and the JVM will make its best effort to achieve it.
+-XX:InitiatingHeapOccupancyPercent=n Percentage of the (entire) heap occupancy to start a concurrent GC cycle. It is used by GCs that trigger a concurrent GC cycle based on the occupancy of the entire heap, not just one of the generations (e.g., G1). A value of 0 denotes 'do constant GC cycles'. The default value is 45.
+-XX:NewRatio=n Ratio of old/new generation sizes. The default value is 2.
+-XX:SurvivorRatio=n Ratio of eden/survivor space size. The default value is 8.
+-XX:MaxTenuringThreshold=n Maximum value for tenuring threshold. The default value is 15.
+-XX:ParallelGCThreads=n Sets the number of threads used during parallel phases of the garbage collectors. The default value varies with the platform on which the JVM is running.
+-XX:ConcGCThreads=n Number of threads concurrent garbage collectors will use. The default value varies with the platform on which the JVM is running.
+-XX:G1ReservePercent=n Sets the amount of heap that is reserved as a false ceiling to reduce the possibility of promotion failure. The default value is 10.
+-XX:G1HeapRegionSize=n With G1 the Java heap is subdivided into uniformly sized regions. This sets the size of the individual sub-divisions. The default value of this parameter is determined ergonomically based upon heap size. The minimum value is 1Mb and the maximum value is 32Mb.
+# Performance Options
+-XX:+AggressiveOpts Turn on point performance compiler optimizations that are expected to be default in upcoming releases. (Introduced in 5.0 update 6.)
+-XX:CompileThreshold=10000 Number of method invocations/branches before compiling [-client: 1,500]
+-XX:LargePageSizeInBytes=4m Sets the large page size used for the Java heap. (Introduced in 1.4.0 update 1.) [amd64: 2m.]
+-XX:MaxHeapFreeRatio=70 Maximum percentage of heap free after GC to avoid shrinking.
+-XX:MaxNewSize=size Maximum size of new generation (in bytes). Since 1.4, MaxNewSize is computed as a function of NewRatio. [1.3.1 Sparc: 32m; 1.3.1 x86: 2.5m.]
+-XX:MaxPermSize=64m Size of the Permanent Generation.  [5.0 and newer: 64 bit VMs are scaled 30% larger; 1.4 amd64: 96m; 1.3.1 -client: 32m.]
+-XX:MinHeapFreeRatio=40 Minimum percentage of heap free after GC to avoid expansion.
+-XX:NewRatio=2 Ratio of old/new generation sizes. [Sparc -client: 8; x86 -server: 8; x86 -client: 12.]-client: 4 (1.3) 8 (1.3.1+), x86: 12]
+-XX:NewSize=2m Default size of new generation (in bytes) [5.0 and newer: 64 bit VMs are scaled 30% larger; x86: 1m; x86, 5.0 and older: 640k]
+-XX:ReservedCodeCacheSize=32m Reserved code cache size (in bytes) - maximum code cache size. [Solaris 64-bit, amd64, and -server x86: 2048m; in 1.5.0_06 and earlier, Solaris 64-bit and amd64: 1024m.]
+-XX:SurvivorRatio=8 Ratio of eden/survivor space size [Solaris amd64: 6; Sparc in 1.3.1: 25; other Solaris platforms in 5.0 and earlier: 32]
+-XX:TargetSurvivorRatio=50 Desired percentage of survivor space used after scavenge.
+-XX:ThreadStackSize=512 Thread Stack Size (in Kbytes). (0 means use default stack size) [Sparc: 512; Solaris x86: 320 (was 256 prior in 5.0 and earlier); Sparc 64 bit: 1024; Linux amd64: 1024 (was 0 in 5.0 and earlier); all others 0.]
+-XX:+UseBiasedLocking Enable biased locking. For more details, see this tuning example. (Introduced in 5.0 update 6.) [5.0: false]
+-XX:+UseFastAccessorMethods Use optimized versions of Get&lt;Primitive&gt;Field.
+-XX:-UseISM Use Intimate Shared Memory. [Not accepted for non-Solaris platforms.] For details, see Intimate Shared Memory.
+-XX:+UseLargePages Use large page memory. (Introduced in 5.0 update 5.) For details, see Java Support for Large Memory Pages.
+-XX:+UseMPSS Use Multiple Page Size Support w/4mb pages for the heap. Do not use with ISM as this replaces the need for ISM. (Introduced in 1.4.0 update 1, Relevant to Solaris 9 and newer.) [1.4.1 and earlier: false]
+-XX:+UseStringCache Enables caching of commonly allocated strings.
+-XX:AllocatePrefetchLines=1 Number of cache lines to load after the last object allocation using prefetch instructions generated in JIT compiled code. Default values are 1 if the last allocated object was an instance and 3 if it was an array. 
+-XX:AllocatePrefetchStyle=1 Generated code style for prefetch instructions.
+0 - no prefetch instructions are generate*d*,
+1 - execute prefetch instructions after each allocation,
+2 - use TLAB allocation watermark pointer to gate when prefetch instructions are executed.
+-XX:+UseCompressedStrings Use a byte[] for Strings which can be represented as pure ASCII. (Introduced in Java 6 Update 21 Performance Release) 
+-XX:+OptimizeStringConcat Optimize String concatenation operations where possible. (Introduced in Java 6 Update 20) 
+# Debugging Options
+-XX:-CITime Prints time spent in JIT Compiler. (Introduced in 1.4.0.)
+-XX:ErrorFile=./hs_err_pid&lt;pid&gt;.log If an error occurs, save the error data to this file. (Introduced in 6.)
+-XX:-ExtendedDTraceProbes Enable performance-impacting dtrace probes. (Introduced in 6. Relevant to Solaris only.)
+-XX:HeapDumpPath=./java_pid&lt;pid&gt;.hprof Path to directory or filename for heap dump. Manageable. (Introduced in 1.4.2 update 12, 5.0 update 7.)
+-XX:-HeapDumpOnOutOfMemoryError Dump heap to file when java.lang.OutOfMemoryError is thrown. Manageable. (Introduced in 1.4.2 update 12, 5.0 update 7.)
+-XX:OnError="&lt;cmd args&gt;;&lt;cmd args&gt;" Run user-defined commands on fatal error. (Introduced in 1.4.2 update 9.)
+-XX:OnOutOfMemoryError="&lt;cmd args&gt;; 
+&lt;cmd args&gt;" Run user-defined commands when an OutOfMemoryError is first thrown. (Introduced in 1.4.2 update 12, 6)
+-XX:-PrintClassHistogram Print a histogram of class instances on Ctrl-Break. Manageable. (Introduced in 1.4.2.) The jmap -histo command provides equivalent functionality.
+-XX:-PrintConcurrentLocks Print java.util.concurrent locks in Ctrl-Break thread dump. Manageable. (Introduced in 6.) The jstack -l command provides equivalent functionality.
+-XX:-PrintCommandLineFlags Print flags that appeared on the command line. (Introduced in 5.0.)
+-XX:-PrintCompilation Print message when a method is compiled.
+-XX:-PrintGC Print messages at garbage collection. Manageable.
+-XX:-PrintGCDetails Print more details at garbage collection. Manageable. (Introduced in 1.4.0.)
+-XX:-PrintGCTimeStamps Print timestamps at garbage collection. Manageable (Introduced in 1.4.0.)
+-XX:-PrintTenuringDistribution Print tenuring age information.
+-XX:-PrintAdaptiveSizePolicy Enables printing of information about adaptive generation sizing.
+-XX:-TraceClassLoading Trace loading of classes.
+-XX:-TraceClassLoadingPreorder Trace all classes loaded in order referenced (not loaded). (Introduced in 1.4.2.)
+-XX:-TraceClassResolution Trace constant pool resolutions. (Introduced in 1.4.2.)
+-XX:-TraceClassUnloading Trace unloading of classes.
+-XX:-TraceLoaderConstraints Trace recording of loader constraints. (Introduced in 6.)
+-XX:+PerfDataSaveToFile Saves jvmstat binary data on exit.
+-XX:ParallelGCThreads=n Sets the number of garbage collection threads in the young and old parallel garbage collectors. The default value varies with the platform on which the JVM is running.
+-XX:+UseCompressedOops Enables the use of compressed pointers (object references represented as 32 bit offsets instead of 64-bit pointers) for optimized 64-bit performance with Java heap sizes less than 32gb.
+-XX:+AlwaysPreTouch Pre-touch the Java heap during JVM initialization. Every page of the heap is thus demand-zeroed during initialization rather than incrementally during application execution.
+-XX:AllocatePrefetchDistance=n Sets the prefetch distance for object allocation. Memory about to be written with the value of new objects is prefetched into cache at this distance (in bytes) beyond the address of the last allocated object. Each Java thread has its own allocation point. The default value varies with the platform on which the JVM is running.
+-XX:InlineSmallCode=n Inline a previously compiled method only if its generated native code size is less than this. The default value varies with the platform on which the JVM is running.
+-XX:MaxInlineSize=35 Maximum bytecode size of a method to be inlined.
+-XX:FreqInlineSize=n Maximum bytecode size of a frequently executed method to be inlined. The default value varies with the platform on which the JVM is running.
+-XX:LoopUnrollLimit=n Unroll loop bodies with server compiler intermediate representation node count less than this value. The limit used by the server compiler is a function of this value, not the actual value. The default value varies with the platform on which the JVM is running.
+-XX:InitialTenuringThreshold=7 Sets the initial tenuring threshold for use in adaptive GC sizing in the parallel young collector. The tenuring threshold is the number of times an object survives a young collection before being promoted to the old, or tenured, generation.
+-XX:MaxTenuringThreshold=n Sets the maximum tenuring threshold for use in adaptive GC sizing. The current largest value is 15. The default value is 15 for the parallel collector and is 4 for CMS.
+-Xloggc:&lt;filename&gt; Log GC verbose output to specified file. The verbose output is controlled by the normal verbose GC flags.
+-XX:-UseGCLogFileRotation Enabled GC log rotation, requires -Xloggc.
+-XX:NumberOfGClogFiles=1 Set the number of files to use when rotating logs, must be &gt;= 1. The rotated log files will use the following naming scheme, &lt;filename&gt;.0, &lt;filename&gt;.1, ..., &lt;filename&gt;.n-1.
+-XX:GCLogFileSize=8K The size of the log file at which point the log will be rotated, must be &gt;= 8K.</t>
+  </si>
+  <si>
+    <t># Man page of JVM (java.exe) covers all options for Window platform:
+http://docs.oracle.com/javase/8/docs/technotes/tools/windows/java.html
+# Option Category
+* __standard options__ like: -jar, -help, -Dproperty=value etc.
+* __non-standard options__ like: -Xdiag, -Xmn512m, -Xmx521m etc.
+* __advanced (runtime control) options__ like: -XX:NativeMemoryTracking=mode, -XX:MaxDirectMemorySize=size, -XX:+ShowMessageBoxOnError etc.. Not recommanded for casual use.</t>
+  </si>
+  <si>
+    <t>-agentlib:libname[=options]
+-agentpath:pathname[=options]
+-client
+-Dproperty=value
+-disableassertions[:[packagename]...|:classname]
+-da[:[packagename]...|:classname]
+-disablesystemassertions
+-dsa
+-enableassertions[:[packagename]...|:classname]
+-ea[:[packagename]...|:classname]
+-enablesystemassertions
+-esa
+-help
+-?
+-jar filename
+-javaagent:jarpath[=options]
+-jre-restrict-search
+-no-jre-restrict-search
+-server
+-showversion
+-splash:imgname
+-verbose:class
+-verbose:gc
+-verbose:jni
+-version
+-version:release</t>
+  </si>
+  <si>
+    <t>-X
+-Xbatch
+-Xbootclasspath:path
+-Xbootclasspath/a:path
+-Xbootclasspath/p:path
+-Xcheck:jni
+-Xcomp
+-Xdebug
+-Xdiag
+-Xfuture
+-Xint
+-Xinternalversion
+-Xloggc:filename
+-Xmaxjitcodesize=size
+-Xmixed
+-Xmnsize
+-Xmssize
+-Xmxsize
+-Xnoclassgc
+-Xprof
+-Xrs
+-Xshare:mode
+-XshowSettings:category
+-Xsssize
+-Xverify:mode</t>
   </si>
 </sst>
 </file>
@@ -4802,10 +4986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B134" sqref="B134"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="32.25" customHeight="1"/>
@@ -6274,6 +6458,50 @@
       </c>
       <c r="C133" s="15" t="s">
         <v>358</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A134" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="B134" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A135" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="B135" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="C135" s="16" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A136" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="B136" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="C136" s="16" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="32.25" customHeight="1">
+      <c r="A137" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="B137" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="C137" s="15" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>